<commit_message>
added scripts and files
</commit_message>
<xml_diff>
--- a/data/dna/dna_metadata.xlsx
+++ b/data/dna/dna_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/moorea_symbiotic_exchange_2023/data/dna/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBDA047-3372-AA41-AE90-51BB7E26C247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B2D9C4-BCDA-5641-9AA7-C23DB38719A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3460" yWindow="820" windowWidth="17180" windowHeight="17560" xr2:uid="{6B87E6CE-126B-8B47-B516-351EEAF1A0B4}"/>
+    <workbookView xWindow="3540" yWindow="820" windowWidth="17180" windowHeight="17560" xr2:uid="{6B87E6CE-126B-8B47-B516-351EEAF1A0B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -38,37 +38,37 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
-    <t>Sample_ID</t>
-  </si>
-  <si>
-    <t>Species</t>
-  </si>
-  <si>
-    <t>Lifestage</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Tube_ID</t>
-  </si>
-  <si>
-    <t>Date_Collected</t>
-  </si>
-  <si>
-    <t>Site</t>
-  </si>
-  <si>
-    <t>Preservation</t>
-  </si>
-  <si>
-    <t>Storage</t>
-  </si>
-  <si>
-    <t>Transport</t>
-  </si>
-  <si>
-    <t>Photo</t>
+    <t>sample_id</t>
+  </si>
+  <si>
+    <t>tube_id</t>
+  </si>
+  <si>
+    <t>photo</t>
+  </si>
+  <si>
+    <t>species</t>
+  </si>
+  <si>
+    <t>lifestage</t>
+  </si>
+  <si>
+    <t>date_collected</t>
+  </si>
+  <si>
+    <t>site</t>
+  </si>
+  <si>
+    <t>preservation</t>
+  </si>
+  <si>
+    <t>storage</t>
+  </si>
+  <si>
+    <t>transport</t>
+  </si>
+  <si>
+    <t>notes</t>
   </si>
 </sst>
 </file>
@@ -438,7 +438,7 @@
   <dimension ref="E1:O1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -456,16 +456,16 @@
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>5</v>
@@ -483,7 +483,7 @@
         <v>9</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added dna sample metadata
</commit_message>
<xml_diff>
--- a/data/dna/dna_metadata.xlsx
+++ b/data/dna/dna_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/moorea_symbiotic_exchange_2023/data/dna/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD0E6E3-B03D-1F49-8687-37992EAA5349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2976A1-B592-6047-94D6-CC7A2E077A4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3540" yWindow="820" windowWidth="24220" windowHeight="17560" xr2:uid="{6B87E6CE-126B-8B47-B516-351EEAF1A0B4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1233" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1331" uniqueCount="276">
   <si>
     <t>sample_id</t>
   </si>
@@ -858,6 +858,12 @@
   </si>
   <si>
     <t>yellow label; IN BAG LABELED POC-R27!</t>
+  </si>
+  <si>
+    <t>Box2</t>
+  </si>
+  <si>
+    <t>Box3</t>
   </si>
 </sst>
 </file>
@@ -894,12 +900,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -914,10 +926,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1235,8 +1249,8 @@
   <dimension ref="A1:L250"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L95" sqref="L95"/>
+      <pane ySplit="1" topLeftCell="A210" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F227" sqref="F227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4461,38 +4475,38 @@
         <v>14</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A142" t="s">
+    <row r="142" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A142" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="B142">
+      <c r="B142" s="3">
         <v>141</v>
       </c>
-      <c r="C142" t="s">
-        <v>13</v>
-      </c>
-      <c r="D142" t="s">
-        <v>11</v>
-      </c>
-      <c r="E142" s="2">
+      <c r="C142" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D142" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E142" s="4">
         <v>20231107</v>
       </c>
-      <c r="F142" t="s">
+      <c r="F142" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G142" t="s">
+      <c r="G142" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H142" t="s">
+      <c r="H142" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I142" t="s">
+      <c r="I142" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K142" t="s">
+      <c r="K142" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L142" t="s">
+      <c r="L142" s="3" t="s">
         <v>14</v>
       </c>
     </row>
@@ -4509,6 +4523,12 @@
       <c r="D143" t="s">
         <v>10</v>
       </c>
+      <c r="E143">
+        <v>2031111</v>
+      </c>
+      <c r="H143" t="s">
+        <v>274</v>
+      </c>
       <c r="L143" t="s">
         <v>272</v>
       </c>
@@ -4526,6 +4546,12 @@
       <c r="D144" t="s">
         <v>10</v>
       </c>
+      <c r="E144">
+        <v>2031111</v>
+      </c>
+      <c r="H144" t="s">
+        <v>274</v>
+      </c>
       <c r="L144" t="s">
         <v>272</v>
       </c>
@@ -4543,6 +4569,12 @@
       <c r="D145" t="s">
         <v>10</v>
       </c>
+      <c r="E145">
+        <v>2031111</v>
+      </c>
+      <c r="H145" t="s">
+        <v>274</v>
+      </c>
       <c r="L145" t="s">
         <v>272</v>
       </c>
@@ -4560,6 +4592,12 @@
       <c r="D146" t="s">
         <v>10</v>
       </c>
+      <c r="E146">
+        <v>2031111</v>
+      </c>
+      <c r="H146" t="s">
+        <v>274</v>
+      </c>
       <c r="L146" t="s">
         <v>272</v>
       </c>
@@ -4577,6 +4615,12 @@
       <c r="D147" t="s">
         <v>10</v>
       </c>
+      <c r="E147">
+        <v>2031111</v>
+      </c>
+      <c r="H147" t="s">
+        <v>274</v>
+      </c>
       <c r="L147" t="s">
         <v>272</v>
       </c>
@@ -4594,6 +4638,12 @@
       <c r="D148" t="s">
         <v>10</v>
       </c>
+      <c r="E148">
+        <v>2031111</v>
+      </c>
+      <c r="H148" t="s">
+        <v>274</v>
+      </c>
       <c r="L148" t="s">
         <v>272</v>
       </c>
@@ -4611,6 +4661,12 @@
       <c r="D149" t="s">
         <v>10</v>
       </c>
+      <c r="E149">
+        <v>2031111</v>
+      </c>
+      <c r="H149" t="s">
+        <v>275</v>
+      </c>
       <c r="L149" t="s">
         <v>272</v>
       </c>
@@ -4628,6 +4684,12 @@
       <c r="D150" t="s">
         <v>10</v>
       </c>
+      <c r="E150">
+        <v>2031111</v>
+      </c>
+      <c r="H150" t="s">
+        <v>274</v>
+      </c>
       <c r="L150" t="s">
         <v>272</v>
       </c>
@@ -4645,6 +4707,12 @@
       <c r="D151" t="s">
         <v>10</v>
       </c>
+      <c r="E151">
+        <v>2031111</v>
+      </c>
+      <c r="H151" t="s">
+        <v>275</v>
+      </c>
       <c r="L151" t="s">
         <v>272</v>
       </c>
@@ -4662,6 +4730,12 @@
       <c r="D152" t="s">
         <v>10</v>
       </c>
+      <c r="E152">
+        <v>2031111</v>
+      </c>
+      <c r="H152" t="s">
+        <v>274</v>
+      </c>
       <c r="L152" t="s">
         <v>272</v>
       </c>
@@ -4679,6 +4753,12 @@
       <c r="D153" t="s">
         <v>10</v>
       </c>
+      <c r="E153">
+        <v>2031111</v>
+      </c>
+      <c r="H153" t="s">
+        <v>274</v>
+      </c>
       <c r="L153" t="s">
         <v>272</v>
       </c>
@@ -4696,6 +4776,12 @@
       <c r="D154" t="s">
         <v>10</v>
       </c>
+      <c r="E154">
+        <v>2031111</v>
+      </c>
+      <c r="H154" t="s">
+        <v>274</v>
+      </c>
       <c r="L154" t="s">
         <v>272</v>
       </c>
@@ -4713,6 +4799,12 @@
       <c r="D155" t="s">
         <v>10</v>
       </c>
+      <c r="E155">
+        <v>2031111</v>
+      </c>
+      <c r="H155" t="s">
+        <v>274</v>
+      </c>
       <c r="L155" t="s">
         <v>272</v>
       </c>
@@ -4730,6 +4822,12 @@
       <c r="D156" t="s">
         <v>10</v>
       </c>
+      <c r="E156">
+        <v>2031111</v>
+      </c>
+      <c r="H156" t="s">
+        <v>274</v>
+      </c>
       <c r="L156" t="s">
         <v>272</v>
       </c>
@@ -4747,6 +4845,12 @@
       <c r="D157" t="s">
         <v>10</v>
       </c>
+      <c r="E157">
+        <v>2031111</v>
+      </c>
+      <c r="H157" t="s">
+        <v>274</v>
+      </c>
       <c r="L157" t="s">
         <v>272</v>
       </c>
@@ -4764,6 +4868,12 @@
       <c r="D158" t="s">
         <v>11</v>
       </c>
+      <c r="E158">
+        <v>2031111</v>
+      </c>
+      <c r="H158" t="s">
+        <v>274</v>
+      </c>
       <c r="L158" t="s">
         <v>272</v>
       </c>
@@ -4781,6 +4891,12 @@
       <c r="D159" t="s">
         <v>11</v>
       </c>
+      <c r="E159">
+        <v>2031111</v>
+      </c>
+      <c r="H159" t="s">
+        <v>274</v>
+      </c>
       <c r="L159" t="s">
         <v>272</v>
       </c>
@@ -4798,6 +4914,12 @@
       <c r="D160" t="s">
         <v>11</v>
       </c>
+      <c r="E160">
+        <v>2031111</v>
+      </c>
+      <c r="H160" t="s">
+        <v>274</v>
+      </c>
       <c r="L160" t="s">
         <v>272</v>
       </c>
@@ -4815,6 +4937,12 @@
       <c r="D161" t="s">
         <v>11</v>
       </c>
+      <c r="E161">
+        <v>2031111</v>
+      </c>
+      <c r="H161" t="s">
+        <v>274</v>
+      </c>
       <c r="L161" t="s">
         <v>272</v>
       </c>
@@ -4832,6 +4960,12 @@
       <c r="D162" t="s">
         <v>11</v>
       </c>
+      <c r="E162">
+        <v>2031111</v>
+      </c>
+      <c r="H162" t="s">
+        <v>274</v>
+      </c>
       <c r="L162" t="s">
         <v>272</v>
       </c>
@@ -4849,6 +4983,12 @@
       <c r="D163" t="s">
         <v>11</v>
       </c>
+      <c r="E163">
+        <v>2031111</v>
+      </c>
+      <c r="H163" t="s">
+        <v>274</v>
+      </c>
       <c r="L163" t="s">
         <v>272</v>
       </c>
@@ -4866,6 +5006,12 @@
       <c r="D164" t="s">
         <v>11</v>
       </c>
+      <c r="E164">
+        <v>2031111</v>
+      </c>
+      <c r="H164" t="s">
+        <v>274</v>
+      </c>
       <c r="L164" t="s">
         <v>272</v>
       </c>
@@ -4883,6 +5029,12 @@
       <c r="D165" t="s">
         <v>11</v>
       </c>
+      <c r="E165">
+        <v>2031111</v>
+      </c>
+      <c r="H165" t="s">
+        <v>274</v>
+      </c>
       <c r="L165" t="s">
         <v>272</v>
       </c>
@@ -4900,6 +5052,12 @@
       <c r="D166" t="s">
         <v>11</v>
       </c>
+      <c r="E166">
+        <v>2031111</v>
+      </c>
+      <c r="H166" t="s">
+        <v>275</v>
+      </c>
       <c r="L166" t="s">
         <v>272</v>
       </c>
@@ -4917,6 +5075,12 @@
       <c r="D167" t="s">
         <v>11</v>
       </c>
+      <c r="E167">
+        <v>2031111</v>
+      </c>
+      <c r="H167" t="s">
+        <v>274</v>
+      </c>
       <c r="L167" t="s">
         <v>272</v>
       </c>
@@ -4934,6 +5098,12 @@
       <c r="D168" t="s">
         <v>11</v>
       </c>
+      <c r="E168">
+        <v>2031111</v>
+      </c>
+      <c r="H168" t="s">
+        <v>275</v>
+      </c>
       <c r="L168" t="s">
         <v>272</v>
       </c>
@@ -4951,6 +5121,12 @@
       <c r="D169" t="s">
         <v>11</v>
       </c>
+      <c r="E169">
+        <v>2031111</v>
+      </c>
+      <c r="H169" t="s">
+        <v>274</v>
+      </c>
       <c r="L169" t="s">
         <v>272</v>
       </c>
@@ -4960,13 +5136,19 @@
         <v>191</v>
       </c>
       <c r="B170">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C170" t="s">
         <v>9</v>
       </c>
       <c r="D170" t="s">
         <v>11</v>
+      </c>
+      <c r="E170">
+        <v>2031111</v>
+      </c>
+      <c r="H170" t="s">
+        <v>275</v>
       </c>
       <c r="L170" t="s">
         <v>272</v>
@@ -4977,13 +5159,19 @@
         <v>192</v>
       </c>
       <c r="B171">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C171" t="s">
         <v>9</v>
       </c>
       <c r="D171" t="s">
         <v>11</v>
+      </c>
+      <c r="E171">
+        <v>2031111</v>
+      </c>
+      <c r="H171" t="s">
+        <v>275</v>
       </c>
       <c r="L171" t="s">
         <v>272</v>
@@ -4994,13 +5182,19 @@
         <v>193</v>
       </c>
       <c r="B172">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C172" t="s">
         <v>9</v>
       </c>
       <c r="D172" t="s">
         <v>11</v>
+      </c>
+      <c r="E172">
+        <v>2031111</v>
+      </c>
+      <c r="H172" t="s">
+        <v>275</v>
       </c>
       <c r="L172" t="s">
         <v>272</v>
@@ -5011,13 +5205,19 @@
         <v>194</v>
       </c>
       <c r="B173">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C173" t="s">
         <v>9</v>
       </c>
       <c r="D173" t="s">
         <v>11</v>
+      </c>
+      <c r="E173">
+        <v>2031111</v>
+      </c>
+      <c r="H173" t="s">
+        <v>274</v>
       </c>
       <c r="L173" t="s">
         <v>272</v>
@@ -5028,13 +5228,19 @@
         <v>195</v>
       </c>
       <c r="B174">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C174" t="s">
         <v>9</v>
       </c>
       <c r="D174" t="s">
         <v>11</v>
+      </c>
+      <c r="E174">
+        <v>2031111</v>
+      </c>
+      <c r="H174" t="s">
+        <v>275</v>
       </c>
       <c r="L174" t="s">
         <v>272</v>
@@ -5045,13 +5251,19 @@
         <v>196</v>
       </c>
       <c r="B175">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C175" t="s">
         <v>9</v>
       </c>
       <c r="D175" t="s">
         <v>11</v>
+      </c>
+      <c r="E175">
+        <v>2031111</v>
+      </c>
+      <c r="H175" t="s">
+        <v>275</v>
       </c>
       <c r="L175" t="s">
         <v>272</v>
@@ -5062,13 +5274,19 @@
         <v>197</v>
       </c>
       <c r="B176">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C176" t="s">
         <v>9</v>
       </c>
       <c r="D176" t="s">
         <v>11</v>
+      </c>
+      <c r="E176">
+        <v>2031111</v>
+      </c>
+      <c r="H176" t="s">
+        <v>274</v>
       </c>
       <c r="L176" t="s">
         <v>272</v>
@@ -5079,13 +5297,19 @@
         <v>198</v>
       </c>
       <c r="B177">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C177" t="s">
         <v>9</v>
       </c>
       <c r="D177" t="s">
         <v>11</v>
+      </c>
+      <c r="E177">
+        <v>2031111</v>
+      </c>
+      <c r="H177" t="s">
+        <v>275</v>
       </c>
       <c r="L177" t="s">
         <v>272</v>
@@ -5096,13 +5320,19 @@
         <v>199</v>
       </c>
       <c r="B178">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C178" t="s">
         <v>9</v>
       </c>
       <c r="D178" t="s">
         <v>11</v>
+      </c>
+      <c r="E178">
+        <v>2031111</v>
+      </c>
+      <c r="H178" t="s">
+        <v>274</v>
       </c>
       <c r="L178" t="s">
         <v>272</v>
@@ -5113,13 +5343,19 @@
         <v>200</v>
       </c>
       <c r="B179">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C179" t="s">
         <v>12</v>
       </c>
       <c r="D179" t="s">
         <v>10</v>
+      </c>
+      <c r="E179">
+        <v>2031111</v>
+      </c>
+      <c r="H179" t="s">
+        <v>274</v>
       </c>
       <c r="L179" t="s">
         <v>272</v>
@@ -5130,13 +5366,19 @@
         <v>201</v>
       </c>
       <c r="B180">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C180" t="s">
         <v>12</v>
       </c>
       <c r="D180" t="s">
         <v>10</v>
+      </c>
+      <c r="E180">
+        <v>2031111</v>
+      </c>
+      <c r="H180" t="s">
+        <v>274</v>
       </c>
       <c r="L180" t="s">
         <v>272</v>
@@ -5147,13 +5389,19 @@
         <v>202</v>
       </c>
       <c r="B181">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C181" t="s">
         <v>12</v>
       </c>
       <c r="D181" t="s">
         <v>10</v>
+      </c>
+      <c r="E181">
+        <v>2031111</v>
+      </c>
+      <c r="H181" t="s">
+        <v>274</v>
       </c>
       <c r="L181" t="s">
         <v>272</v>
@@ -5164,13 +5412,19 @@
         <v>203</v>
       </c>
       <c r="B182">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C182" t="s">
         <v>12</v>
       </c>
       <c r="D182" t="s">
         <v>10</v>
+      </c>
+      <c r="E182">
+        <v>2031111</v>
+      </c>
+      <c r="H182" t="s">
+        <v>274</v>
       </c>
       <c r="L182" t="s">
         <v>272</v>
@@ -5181,13 +5435,19 @@
         <v>204</v>
       </c>
       <c r="B183">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C183" t="s">
         <v>12</v>
       </c>
       <c r="D183" t="s">
         <v>10</v>
+      </c>
+      <c r="E183">
+        <v>2031111</v>
+      </c>
+      <c r="H183" t="s">
+        <v>274</v>
       </c>
       <c r="L183" t="s">
         <v>272</v>
@@ -5198,13 +5458,19 @@
         <v>205</v>
       </c>
       <c r="B184">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C184" t="s">
         <v>12</v>
       </c>
       <c r="D184" t="s">
         <v>10</v>
+      </c>
+      <c r="E184">
+        <v>2031111</v>
+      </c>
+      <c r="H184" t="s">
+        <v>274</v>
       </c>
       <c r="L184" t="s">
         <v>272</v>
@@ -5215,13 +5481,19 @@
         <v>206</v>
       </c>
       <c r="B185">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C185" t="s">
         <v>12</v>
       </c>
       <c r="D185" t="s">
         <v>10</v>
+      </c>
+      <c r="E185">
+        <v>2031111</v>
+      </c>
+      <c r="H185" t="s">
+        <v>274</v>
       </c>
       <c r="L185" t="s">
         <v>272</v>
@@ -5232,13 +5504,19 @@
         <v>207</v>
       </c>
       <c r="B186">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C186" t="s">
         <v>12</v>
       </c>
       <c r="D186" t="s">
         <v>10</v>
+      </c>
+      <c r="E186">
+        <v>2031111</v>
+      </c>
+      <c r="H186" t="s">
+        <v>274</v>
       </c>
       <c r="L186" t="s">
         <v>272</v>
@@ -5249,13 +5527,19 @@
         <v>208</v>
       </c>
       <c r="B187">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C187" t="s">
         <v>12</v>
       </c>
       <c r="D187" t="s">
         <v>10</v>
+      </c>
+      <c r="E187">
+        <v>2031111</v>
+      </c>
+      <c r="H187" t="s">
+        <v>274</v>
       </c>
       <c r="L187" t="s">
         <v>272</v>
@@ -5266,13 +5550,19 @@
         <v>209</v>
       </c>
       <c r="B188">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C188" t="s">
         <v>12</v>
       </c>
       <c r="D188" t="s">
         <v>10</v>
+      </c>
+      <c r="E188">
+        <v>2031111</v>
+      </c>
+      <c r="H188" t="s">
+        <v>274</v>
       </c>
       <c r="L188" t="s">
         <v>272</v>
@@ -5283,13 +5573,19 @@
         <v>210</v>
       </c>
       <c r="B189">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C189" t="s">
         <v>12</v>
       </c>
       <c r="D189" t="s">
         <v>10</v>
+      </c>
+      <c r="E189">
+        <v>2031111</v>
+      </c>
+      <c r="H189" t="s">
+        <v>274</v>
       </c>
       <c r="L189" t="s">
         <v>272</v>
@@ -5300,13 +5596,19 @@
         <v>211</v>
       </c>
       <c r="B190">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C190" t="s">
         <v>12</v>
       </c>
       <c r="D190" t="s">
         <v>10</v>
+      </c>
+      <c r="E190">
+        <v>2031111</v>
+      </c>
+      <c r="H190" t="s">
+        <v>274</v>
       </c>
       <c r="L190" t="s">
         <v>272</v>
@@ -5317,13 +5619,19 @@
         <v>212</v>
       </c>
       <c r="B191">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C191" t="s">
         <v>12</v>
       </c>
       <c r="D191" t="s">
         <v>10</v>
+      </c>
+      <c r="E191">
+        <v>2031111</v>
+      </c>
+      <c r="H191" t="s">
+        <v>274</v>
       </c>
       <c r="L191" t="s">
         <v>272</v>
@@ -5334,13 +5642,19 @@
         <v>213</v>
       </c>
       <c r="B192">
-        <v>191</v>
+        <v>228</v>
       </c>
       <c r="C192" t="s">
         <v>12</v>
       </c>
       <c r="D192" t="s">
         <v>10</v>
+      </c>
+      <c r="E192">
+        <v>2031111</v>
+      </c>
+      <c r="H192" t="s">
+        <v>274</v>
       </c>
       <c r="L192" t="s">
         <v>272</v>
@@ -5351,13 +5665,19 @@
         <v>214</v>
       </c>
       <c r="B193">
-        <v>192</v>
+        <v>229</v>
       </c>
       <c r="C193" t="s">
         <v>12</v>
       </c>
       <c r="D193" t="s">
         <v>10</v>
+      </c>
+      <c r="E193">
+        <v>2031111</v>
+      </c>
+      <c r="H193" t="s">
+        <v>274</v>
       </c>
       <c r="L193" t="s">
         <v>272</v>
@@ -5368,13 +5688,19 @@
         <v>215</v>
       </c>
       <c r="B194">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C194" t="s">
         <v>12</v>
       </c>
       <c r="D194" t="s">
         <v>11</v>
+      </c>
+      <c r="E194">
+        <v>2031111</v>
+      </c>
+      <c r="H194" t="s">
+        <v>274</v>
       </c>
       <c r="L194" t="s">
         <v>272</v>
@@ -5385,13 +5711,19 @@
         <v>216</v>
       </c>
       <c r="B195">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C195" t="s">
         <v>12</v>
       </c>
       <c r="D195" t="s">
         <v>11</v>
+      </c>
+      <c r="E195">
+        <v>2031111</v>
+      </c>
+      <c r="H195" t="s">
+        <v>274</v>
       </c>
       <c r="L195" t="s">
         <v>272</v>
@@ -5402,13 +5734,19 @@
         <v>217</v>
       </c>
       <c r="B196">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C196" t="s">
         <v>12</v>
       </c>
       <c r="D196" t="s">
         <v>11</v>
+      </c>
+      <c r="E196">
+        <v>2031111</v>
+      </c>
+      <c r="H196" t="s">
+        <v>274</v>
       </c>
       <c r="L196" t="s">
         <v>272</v>
@@ -5419,13 +5757,19 @@
         <v>218</v>
       </c>
       <c r="B197">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C197" t="s">
         <v>12</v>
       </c>
       <c r="D197" t="s">
         <v>11</v>
+      </c>
+      <c r="E197">
+        <v>2031111</v>
+      </c>
+      <c r="H197" t="s">
+        <v>274</v>
       </c>
       <c r="L197" t="s">
         <v>272</v>
@@ -5436,13 +5780,19 @@
         <v>219</v>
       </c>
       <c r="B198">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C198" t="s">
         <v>12</v>
       </c>
       <c r="D198" t="s">
         <v>11</v>
+      </c>
+      <c r="E198">
+        <v>2031111</v>
+      </c>
+      <c r="H198" t="s">
+        <v>274</v>
       </c>
       <c r="L198" t="s">
         <v>272</v>
@@ -5450,16 +5800,22 @@
     </row>
     <row r="199" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B199">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C199" t="s">
         <v>12</v>
       </c>
       <c r="D199" t="s">
         <v>11</v>
+      </c>
+      <c r="E199">
+        <v>2023111</v>
+      </c>
+      <c r="H199" t="s">
+        <v>274</v>
       </c>
       <c r="L199" t="s">
         <v>272</v>
@@ -5467,16 +5823,22 @@
     </row>
     <row r="200" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B200">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C200" t="s">
         <v>12</v>
       </c>
       <c r="D200" t="s">
         <v>11</v>
+      </c>
+      <c r="E200">
+        <v>2023111</v>
+      </c>
+      <c r="H200" t="s">
+        <v>274</v>
       </c>
       <c r="L200" t="s">
         <v>272</v>
@@ -5484,16 +5846,22 @@
     </row>
     <row r="201" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B201">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C201" t="s">
         <v>12</v>
       </c>
       <c r="D201" t="s">
         <v>11</v>
+      </c>
+      <c r="E201">
+        <v>2031111</v>
+      </c>
+      <c r="H201" t="s">
+        <v>274</v>
       </c>
       <c r="L201" t="s">
         <v>272</v>
@@ -5504,13 +5872,19 @@
         <v>223</v>
       </c>
       <c r="B202">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C202" t="s">
         <v>12</v>
       </c>
       <c r="D202" t="s">
         <v>11</v>
+      </c>
+      <c r="E202">
+        <v>2031111</v>
+      </c>
+      <c r="H202" t="s">
+        <v>274</v>
       </c>
       <c r="L202" t="s">
         <v>272</v>
@@ -5521,13 +5895,19 @@
         <v>224</v>
       </c>
       <c r="B203">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C203" t="s">
         <v>12</v>
       </c>
       <c r="D203" t="s">
         <v>11</v>
+      </c>
+      <c r="E203">
+        <v>2031111</v>
+      </c>
+      <c r="H203" t="s">
+        <v>274</v>
       </c>
       <c r="L203" t="s">
         <v>272</v>
@@ -5538,13 +5918,19 @@
         <v>225</v>
       </c>
       <c r="B204">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C204" t="s">
         <v>12</v>
       </c>
       <c r="D204" t="s">
         <v>11</v>
+      </c>
+      <c r="E204">
+        <v>2031111</v>
+      </c>
+      <c r="H204" t="s">
+        <v>274</v>
       </c>
       <c r="L204" t="s">
         <v>272</v>
@@ -5555,13 +5941,19 @@
         <v>226</v>
       </c>
       <c r="B205">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C205" t="s">
         <v>12</v>
       </c>
       <c r="D205" t="s">
         <v>11</v>
+      </c>
+      <c r="E205">
+        <v>2031111</v>
+      </c>
+      <c r="H205" t="s">
+        <v>274</v>
       </c>
       <c r="L205" t="s">
         <v>272</v>
@@ -5572,13 +5964,19 @@
         <v>227</v>
       </c>
       <c r="B206">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C206" t="s">
         <v>12</v>
       </c>
       <c r="D206" t="s">
         <v>11</v>
+      </c>
+      <c r="E206">
+        <v>2031111</v>
+      </c>
+      <c r="H206" t="s">
+        <v>274</v>
       </c>
       <c r="L206" t="s">
         <v>272</v>
@@ -5589,13 +5987,19 @@
         <v>228</v>
       </c>
       <c r="B207">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C207" t="s">
         <v>12</v>
       </c>
       <c r="D207" t="s">
         <v>11</v>
+      </c>
+      <c r="E207">
+        <v>2031111</v>
+      </c>
+      <c r="H207" t="s">
+        <v>274</v>
       </c>
       <c r="L207" t="s">
         <v>272</v>
@@ -5606,13 +6010,19 @@
         <v>229</v>
       </c>
       <c r="B208">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C208" t="s">
         <v>12</v>
       </c>
       <c r="D208" t="s">
         <v>11</v>
+      </c>
+      <c r="E208">
+        <v>2031111</v>
+      </c>
+      <c r="H208" t="s">
+        <v>274</v>
       </c>
       <c r="L208" t="s">
         <v>272</v>
@@ -5623,13 +6033,19 @@
         <v>230</v>
       </c>
       <c r="B209">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C209" t="s">
         <v>12</v>
       </c>
       <c r="D209" t="s">
         <v>11</v>
+      </c>
+      <c r="E209">
+        <v>2031111</v>
+      </c>
+      <c r="H209" t="s">
+        <v>274</v>
       </c>
       <c r="L209" t="s">
         <v>272</v>
@@ -5640,13 +6056,19 @@
         <v>231</v>
       </c>
       <c r="B210">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C210" t="s">
         <v>12</v>
       </c>
       <c r="D210" t="s">
         <v>11</v>
+      </c>
+      <c r="E210">
+        <v>2031111</v>
+      </c>
+      <c r="H210" t="s">
+        <v>274</v>
       </c>
       <c r="L210" t="s">
         <v>272</v>
@@ -5657,13 +6079,19 @@
         <v>232</v>
       </c>
       <c r="B211">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C211" t="s">
         <v>12</v>
       </c>
       <c r="D211" t="s">
         <v>11</v>
+      </c>
+      <c r="E211">
+        <v>2031111</v>
+      </c>
+      <c r="H211" t="s">
+        <v>274</v>
       </c>
       <c r="L211" t="s">
         <v>272</v>
@@ -5674,13 +6102,19 @@
         <v>233</v>
       </c>
       <c r="B212">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C212" t="s">
         <v>12</v>
       </c>
       <c r="D212" t="s">
         <v>11</v>
+      </c>
+      <c r="E212">
+        <v>2031111</v>
+      </c>
+      <c r="H212" t="s">
+        <v>274</v>
       </c>
       <c r="L212" t="s">
         <v>272</v>
@@ -5691,13 +6125,19 @@
         <v>234</v>
       </c>
       <c r="B213">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C213" t="s">
         <v>12</v>
       </c>
       <c r="D213" t="s">
         <v>11</v>
+      </c>
+      <c r="E213">
+        <v>2031111</v>
+      </c>
+      <c r="H213" t="s">
+        <v>274</v>
       </c>
       <c r="L213" t="s">
         <v>272</v>
@@ -5708,13 +6148,19 @@
         <v>235</v>
       </c>
       <c r="B214">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C214" t="s">
         <v>12</v>
       </c>
       <c r="D214" t="s">
         <v>11</v>
+      </c>
+      <c r="E214">
+        <v>2031111</v>
+      </c>
+      <c r="H214" t="s">
+        <v>274</v>
       </c>
       <c r="L214" t="s">
         <v>272</v>
@@ -5725,13 +6171,19 @@
         <v>236</v>
       </c>
       <c r="B215">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C215" t="s">
         <v>13</v>
       </c>
       <c r="D215" t="s">
         <v>10</v>
+      </c>
+      <c r="E215">
+        <v>2031111</v>
+      </c>
+      <c r="H215" t="s">
+        <v>275</v>
       </c>
       <c r="L215" t="s">
         <v>272</v>
@@ -5742,13 +6194,19 @@
         <v>237</v>
       </c>
       <c r="B216">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C216" t="s">
         <v>13</v>
       </c>
       <c r="D216" t="s">
         <v>10</v>
+      </c>
+      <c r="E216">
+        <v>2031111</v>
+      </c>
+      <c r="H216" t="s">
+        <v>274</v>
       </c>
       <c r="L216" t="s">
         <v>272</v>
@@ -5759,13 +6217,19 @@
         <v>238</v>
       </c>
       <c r="B217">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C217" t="s">
         <v>13</v>
       </c>
       <c r="D217" t="s">
         <v>10</v>
+      </c>
+      <c r="E217">
+        <v>2031111</v>
+      </c>
+      <c r="H217" t="s">
+        <v>275</v>
       </c>
       <c r="L217" t="s">
         <v>272</v>
@@ -5776,13 +6240,19 @@
         <v>239</v>
       </c>
       <c r="B218">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C218" t="s">
         <v>13</v>
       </c>
       <c r="D218" t="s">
         <v>10</v>
+      </c>
+      <c r="E218">
+        <v>2031111</v>
+      </c>
+      <c r="H218" t="s">
+        <v>275</v>
       </c>
       <c r="L218" t="s">
         <v>272</v>
@@ -5793,13 +6263,19 @@
         <v>240</v>
       </c>
       <c r="B219">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C219" t="s">
         <v>13</v>
       </c>
       <c r="D219" t="s">
         <v>10</v>
+      </c>
+      <c r="E219">
+        <v>2031111</v>
+      </c>
+      <c r="H219" t="s">
+        <v>274</v>
       </c>
       <c r="L219" t="s">
         <v>272</v>
@@ -5810,13 +6286,19 @@
         <v>241</v>
       </c>
       <c r="B220">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C220" t="s">
         <v>13</v>
       </c>
       <c r="D220" t="s">
         <v>10</v>
+      </c>
+      <c r="E220">
+        <v>2031111</v>
+      </c>
+      <c r="H220" t="s">
+        <v>275</v>
       </c>
       <c r="L220" t="s">
         <v>272</v>
@@ -5827,7 +6309,7 @@
         <v>242</v>
       </c>
       <c r="B221">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C221" t="s">
         <v>13</v>
@@ -5844,7 +6326,7 @@
         <v>243</v>
       </c>
       <c r="B222">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C222" t="s">
         <v>13</v>
@@ -5861,7 +6343,7 @@
         <v>244</v>
       </c>
       <c r="B223">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C223" t="s">
         <v>13</v>
@@ -5878,7 +6360,7 @@
         <v>245</v>
       </c>
       <c r="B224">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C224" t="s">
         <v>13</v>
@@ -5895,7 +6377,7 @@
         <v>246</v>
       </c>
       <c r="B225">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C225" t="s">
         <v>13</v>
@@ -5912,7 +6394,7 @@
         <v>247</v>
       </c>
       <c r="B226">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C226" t="s">
         <v>13</v>
@@ -5929,13 +6411,19 @@
         <v>248</v>
       </c>
       <c r="B227">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C227" t="s">
         <v>13</v>
       </c>
       <c r="D227" t="s">
         <v>10</v>
+      </c>
+      <c r="E227">
+        <v>2031111</v>
+      </c>
+      <c r="H227" t="s">
+        <v>274</v>
       </c>
       <c r="L227" t="s">
         <v>272</v>
@@ -5946,13 +6434,19 @@
         <v>249</v>
       </c>
       <c r="B228">
-        <v>227</v>
+        <v>192</v>
       </c>
       <c r="C228" t="s">
         <v>13</v>
       </c>
       <c r="D228" t="s">
         <v>10</v>
+      </c>
+      <c r="E228">
+        <v>2031111</v>
+      </c>
+      <c r="H228" t="s">
+        <v>275</v>
       </c>
       <c r="L228" t="s">
         <v>272</v>
@@ -5963,13 +6457,19 @@
         <v>250</v>
       </c>
       <c r="B229">
-        <v>228</v>
+        <v>193</v>
       </c>
       <c r="C229" t="s">
         <v>13</v>
       </c>
       <c r="D229" t="s">
         <v>10</v>
+      </c>
+      <c r="E229">
+        <v>2031111</v>
+      </c>
+      <c r="H229" t="s">
+        <v>274</v>
       </c>
       <c r="L229" t="s">
         <v>272</v>
@@ -5980,13 +6480,19 @@
         <v>251</v>
       </c>
       <c r="B230">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C230" t="s">
         <v>13</v>
       </c>
       <c r="D230" t="s">
         <v>11</v>
+      </c>
+      <c r="E230">
+        <v>2031111</v>
+      </c>
+      <c r="H230" t="s">
+        <v>274</v>
       </c>
       <c r="L230" t="s">
         <v>272</v>
@@ -5997,13 +6503,19 @@
         <v>252</v>
       </c>
       <c r="B231">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C231" t="s">
         <v>13</v>
       </c>
       <c r="D231" t="s">
         <v>11</v>
+      </c>
+      <c r="E231">
+        <v>2031111</v>
+      </c>
+      <c r="H231" t="s">
+        <v>274</v>
       </c>
       <c r="L231" t="s">
         <v>272</v>
@@ -6014,13 +6526,19 @@
         <v>253</v>
       </c>
       <c r="B232">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C232" t="s">
         <v>13</v>
       </c>
       <c r="D232" t="s">
         <v>11</v>
+      </c>
+      <c r="E232">
+        <v>2031111</v>
+      </c>
+      <c r="H232" t="s">
+        <v>274</v>
       </c>
       <c r="L232" t="s">
         <v>272</v>
@@ -6031,13 +6549,19 @@
         <v>254</v>
       </c>
       <c r="B233">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C233" t="s">
         <v>13</v>
       </c>
       <c r="D233" t="s">
         <v>11</v>
+      </c>
+      <c r="E233">
+        <v>2031111</v>
+      </c>
+      <c r="H233" t="s">
+        <v>274</v>
       </c>
       <c r="L233" t="s">
         <v>272</v>
@@ -6048,13 +6572,19 @@
         <v>255</v>
       </c>
       <c r="B234">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C234" t="s">
         <v>13</v>
       </c>
       <c r="D234" t="s">
         <v>11</v>
+      </c>
+      <c r="E234">
+        <v>2031111</v>
+      </c>
+      <c r="H234" t="s">
+        <v>274</v>
       </c>
       <c r="L234" t="s">
         <v>272</v>
@@ -6065,13 +6595,19 @@
         <v>256</v>
       </c>
       <c r="B235">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C235" t="s">
         <v>13</v>
       </c>
       <c r="D235" t="s">
         <v>11</v>
+      </c>
+      <c r="E235">
+        <v>2031111</v>
+      </c>
+      <c r="H235" t="s">
+        <v>274</v>
       </c>
       <c r="L235" t="s">
         <v>272</v>
@@ -6082,13 +6618,19 @@
         <v>257</v>
       </c>
       <c r="B236">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C236" t="s">
         <v>13</v>
       </c>
       <c r="D236" t="s">
         <v>11</v>
+      </c>
+      <c r="E236">
+        <v>2031111</v>
+      </c>
+      <c r="H236" t="s">
+        <v>275</v>
       </c>
       <c r="L236" t="s">
         <v>272</v>
@@ -6099,13 +6641,19 @@
         <v>258</v>
       </c>
       <c r="B237">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C237" t="s">
         <v>13</v>
       </c>
       <c r="D237" t="s">
         <v>11</v>
+      </c>
+      <c r="E237">
+        <v>2031111</v>
+      </c>
+      <c r="H237" t="s">
+        <v>274</v>
       </c>
       <c r="L237" t="s">
         <v>272</v>
@@ -6116,13 +6664,19 @@
         <v>259</v>
       </c>
       <c r="B238">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C238" t="s">
         <v>13</v>
       </c>
       <c r="D238" t="s">
         <v>11</v>
+      </c>
+      <c r="E238">
+        <v>2031111</v>
+      </c>
+      <c r="H238" t="s">
+        <v>274</v>
       </c>
       <c r="L238" t="s">
         <v>272</v>
@@ -6133,13 +6687,19 @@
         <v>260</v>
       </c>
       <c r="B239">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C239" t="s">
         <v>13</v>
       </c>
       <c r="D239" t="s">
         <v>11</v>
+      </c>
+      <c r="E239">
+        <v>2031111</v>
+      </c>
+      <c r="H239" t="s">
+        <v>274</v>
       </c>
       <c r="L239" t="s">
         <v>272</v>
@@ -6150,13 +6710,19 @@
         <v>261</v>
       </c>
       <c r="B240">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C240" t="s">
         <v>13</v>
       </c>
       <c r="D240" t="s">
         <v>11</v>
+      </c>
+      <c r="E240">
+        <v>2031111</v>
+      </c>
+      <c r="H240" t="s">
+        <v>275</v>
       </c>
       <c r="L240" t="s">
         <v>272</v>
@@ -6167,13 +6733,19 @@
         <v>262</v>
       </c>
       <c r="B241">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="C241" t="s">
         <v>13</v>
       </c>
       <c r="D241" t="s">
         <v>11</v>
+      </c>
+      <c r="E241">
+        <v>2031111</v>
+      </c>
+      <c r="H241" t="s">
+        <v>274</v>
       </c>
       <c r="L241" t="s">
         <v>272</v>
@@ -6184,13 +6756,19 @@
         <v>263</v>
       </c>
       <c r="B242">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="C242" t="s">
         <v>13</v>
       </c>
       <c r="D242" t="s">
         <v>11</v>
+      </c>
+      <c r="E242">
+        <v>2031111</v>
+      </c>
+      <c r="H242" t="s">
+        <v>274</v>
       </c>
       <c r="L242" t="s">
         <v>272</v>
@@ -6201,7 +6779,7 @@
         <v>264</v>
       </c>
       <c r="B243">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C243" t="s">
         <v>13</v>
@@ -6218,7 +6796,7 @@
         <v>265</v>
       </c>
       <c r="B244">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="C244" t="s">
         <v>13</v>
@@ -6235,7 +6813,7 @@
         <v>266</v>
       </c>
       <c r="B245">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C245" t="s">
         <v>13</v>
@@ -6252,7 +6830,7 @@
         <v>267</v>
       </c>
       <c r="B246">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C246" t="s">
         <v>13</v>
@@ -6269,13 +6847,19 @@
         <v>268</v>
       </c>
       <c r="B247">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C247" t="s">
         <v>13</v>
       </c>
       <c r="D247" t="s">
         <v>11</v>
+      </c>
+      <c r="E247">
+        <v>2031111</v>
+      </c>
+      <c r="H247" t="s">
+        <v>274</v>
       </c>
       <c r="L247" t="s">
         <v>272</v>
@@ -6286,13 +6870,19 @@
         <v>269</v>
       </c>
       <c r="B248">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C248" t="s">
         <v>13</v>
       </c>
       <c r="D248" t="s">
         <v>11</v>
+      </c>
+      <c r="E248">
+        <v>2031111</v>
+      </c>
+      <c r="H248" t="s">
+        <v>274</v>
       </c>
       <c r="L248" t="s">
         <v>272</v>
@@ -6303,13 +6893,19 @@
         <v>270</v>
       </c>
       <c r="B249">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C249" t="s">
         <v>13</v>
       </c>
       <c r="D249" t="s">
         <v>11</v>
+      </c>
+      <c r="E249">
+        <v>2031111</v>
+      </c>
+      <c r="H249" t="s">
+        <v>274</v>
       </c>
       <c r="L249" t="s">
         <v>272</v>
@@ -6320,13 +6916,19 @@
         <v>271</v>
       </c>
       <c r="B250">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C250" t="s">
         <v>13</v>
       </c>
       <c r="D250" t="s">
         <v>11</v>
+      </c>
+      <c r="E250">
+        <v>2031111</v>
+      </c>
+      <c r="H250" t="s">
+        <v>274</v>
       </c>
       <c r="L250" t="s">
         <v>272</v>

</xml_diff>

<commit_message>
added loggers and updated metadata
</commit_message>
<xml_diff>
--- a/data/dna/dna_metadata.xlsx
+++ b/data/dna/dna_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/moorea_symbiotic_exchange_2023/data/dna/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2976A1-B592-6047-94D6-CC7A2E077A4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7724F164-D563-D84F-AFE5-7CB279B88C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3540" yWindow="820" windowWidth="24220" windowHeight="17560" xr2:uid="{6B87E6CE-126B-8B47-B516-351EEAF1A0B4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1331" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1751" uniqueCount="278">
   <si>
     <t>sample_id</t>
   </si>
@@ -864,6 +864,12 @@
   </si>
   <si>
     <t>Box3</t>
+  </si>
+  <si>
+    <t>PR Rates</t>
+  </si>
+  <si>
+    <t>Isotopes</t>
   </si>
 </sst>
 </file>
@@ -1249,8 +1255,8 @@
   <dimension ref="A1:L250"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A210" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F227" sqref="F227"/>
+      <pane ySplit="1" topLeftCell="A211" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F242" sqref="F242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1316,6 +1322,9 @@
       <c r="D2" t="s">
         <v>10</v>
       </c>
+      <c r="F2" t="s">
+        <v>276</v>
+      </c>
       <c r="L2" t="s">
         <v>14</v>
       </c>
@@ -1333,6 +1342,9 @@
       <c r="D3" t="s">
         <v>10</v>
       </c>
+      <c r="F3" t="s">
+        <v>276</v>
+      </c>
       <c r="L3" t="s">
         <v>14</v>
       </c>
@@ -1350,6 +1362,9 @@
       <c r="D4" t="s">
         <v>10</v>
       </c>
+      <c r="F4" t="s">
+        <v>276</v>
+      </c>
       <c r="L4" t="s">
         <v>14</v>
       </c>
@@ -1367,6 +1382,9 @@
       <c r="D5" t="s">
         <v>10</v>
       </c>
+      <c r="F5" t="s">
+        <v>276</v>
+      </c>
       <c r="L5" t="s">
         <v>14</v>
       </c>
@@ -1384,6 +1402,9 @@
       <c r="D6" t="s">
         <v>10</v>
       </c>
+      <c r="F6" t="s">
+        <v>276</v>
+      </c>
       <c r="L6" t="s">
         <v>14</v>
       </c>
@@ -1401,6 +1422,9 @@
       <c r="D7" t="s">
         <v>10</v>
       </c>
+      <c r="F7" t="s">
+        <v>276</v>
+      </c>
       <c r="L7" t="s">
         <v>14</v>
       </c>
@@ -1418,6 +1442,9 @@
       <c r="D8" t="s">
         <v>10</v>
       </c>
+      <c r="F8" t="s">
+        <v>276</v>
+      </c>
       <c r="L8" t="s">
         <v>14</v>
       </c>
@@ -1435,6 +1462,9 @@
       <c r="D9" t="s">
         <v>10</v>
       </c>
+      <c r="F9" t="s">
+        <v>276</v>
+      </c>
       <c r="L9" t="s">
         <v>14</v>
       </c>
@@ -1452,6 +1482,9 @@
       <c r="D10" t="s">
         <v>10</v>
       </c>
+      <c r="F10" t="s">
+        <v>276</v>
+      </c>
       <c r="L10" t="s">
         <v>14</v>
       </c>
@@ -1469,6 +1502,9 @@
       <c r="D11" t="s">
         <v>10</v>
       </c>
+      <c r="F11" t="s">
+        <v>276</v>
+      </c>
       <c r="L11" t="s">
         <v>14</v>
       </c>
@@ -1486,6 +1522,9 @@
       <c r="D12" t="s">
         <v>10</v>
       </c>
+      <c r="F12" t="s">
+        <v>276</v>
+      </c>
       <c r="L12" t="s">
         <v>14</v>
       </c>
@@ -1503,6 +1542,9 @@
       <c r="D13" t="s">
         <v>10</v>
       </c>
+      <c r="F13" t="s">
+        <v>276</v>
+      </c>
       <c r="L13" t="s">
         <v>14</v>
       </c>
@@ -1520,6 +1562,9 @@
       <c r="D14" t="s">
         <v>11</v>
       </c>
+      <c r="F14" t="s">
+        <v>276</v>
+      </c>
       <c r="L14" t="s">
         <v>14</v>
       </c>
@@ -1537,6 +1582,9 @@
       <c r="D15" t="s">
         <v>11</v>
       </c>
+      <c r="F15" t="s">
+        <v>276</v>
+      </c>
       <c r="L15" t="s">
         <v>14</v>
       </c>
@@ -1554,6 +1602,9 @@
       <c r="D16" t="s">
         <v>11</v>
       </c>
+      <c r="F16" t="s">
+        <v>276</v>
+      </c>
       <c r="L16" t="s">
         <v>14</v>
       </c>
@@ -1571,6 +1622,9 @@
       <c r="D17" t="s">
         <v>11</v>
       </c>
+      <c r="F17" t="s">
+        <v>276</v>
+      </c>
       <c r="L17" t="s">
         <v>14</v>
       </c>
@@ -1588,6 +1642,9 @@
       <c r="D18" t="s">
         <v>11</v>
       </c>
+      <c r="F18" t="s">
+        <v>276</v>
+      </c>
       <c r="L18" t="s">
         <v>14</v>
       </c>
@@ -1605,6 +1662,9 @@
       <c r="D19" t="s">
         <v>11</v>
       </c>
+      <c r="F19" t="s">
+        <v>276</v>
+      </c>
       <c r="L19" t="s">
         <v>14</v>
       </c>
@@ -1622,6 +1682,9 @@
       <c r="D20" t="s">
         <v>11</v>
       </c>
+      <c r="F20" t="s">
+        <v>276</v>
+      </c>
       <c r="L20" t="s">
         <v>14</v>
       </c>
@@ -1639,6 +1702,9 @@
       <c r="D21" t="s">
         <v>11</v>
       </c>
+      <c r="F21" t="s">
+        <v>276</v>
+      </c>
       <c r="L21" t="s">
         <v>14</v>
       </c>
@@ -1656,6 +1722,9 @@
       <c r="D22" t="s">
         <v>11</v>
       </c>
+      <c r="F22" t="s">
+        <v>276</v>
+      </c>
       <c r="L22" t="s">
         <v>14</v>
       </c>
@@ -1673,6 +1742,9 @@
       <c r="D23" t="s">
         <v>11</v>
       </c>
+      <c r="F23" t="s">
+        <v>276</v>
+      </c>
       <c r="L23" t="s">
         <v>14</v>
       </c>
@@ -1690,6 +1762,9 @@
       <c r="D24" t="s">
         <v>11</v>
       </c>
+      <c r="F24" t="s">
+        <v>276</v>
+      </c>
       <c r="L24" t="s">
         <v>14</v>
       </c>
@@ -1707,6 +1782,9 @@
       <c r="D25" t="s">
         <v>11</v>
       </c>
+      <c r="F25" t="s">
+        <v>276</v>
+      </c>
       <c r="L25" t="s">
         <v>14</v>
       </c>
@@ -1724,6 +1802,9 @@
       <c r="D26" t="s">
         <v>11</v>
       </c>
+      <c r="F26" t="s">
+        <v>276</v>
+      </c>
       <c r="L26" t="s">
         <v>14</v>
       </c>
@@ -1741,6 +1822,9 @@
       <c r="D27" t="s">
         <v>11</v>
       </c>
+      <c r="F27" t="s">
+        <v>276</v>
+      </c>
       <c r="L27" t="s">
         <v>14</v>
       </c>
@@ -1758,6 +1842,9 @@
       <c r="D28" t="s">
         <v>11</v>
       </c>
+      <c r="F28" t="s">
+        <v>276</v>
+      </c>
       <c r="L28" t="s">
         <v>14</v>
       </c>
@@ -1775,6 +1862,9 @@
       <c r="D29" t="s">
         <v>11</v>
       </c>
+      <c r="F29" t="s">
+        <v>276</v>
+      </c>
       <c r="L29" t="s">
         <v>14</v>
       </c>
@@ -1792,6 +1882,9 @@
       <c r="D30" t="s">
         <v>11</v>
       </c>
+      <c r="F30" t="s">
+        <v>276</v>
+      </c>
       <c r="L30" t="s">
         <v>14</v>
       </c>
@@ -1809,6 +1902,9 @@
       <c r="D31" t="s">
         <v>11</v>
       </c>
+      <c r="F31" t="s">
+        <v>276</v>
+      </c>
       <c r="L31" t="s">
         <v>14</v>
       </c>
@@ -1826,6 +1922,9 @@
       <c r="D32" t="s">
         <v>11</v>
       </c>
+      <c r="F32" t="s">
+        <v>276</v>
+      </c>
       <c r="L32" t="s">
         <v>14</v>
       </c>
@@ -1843,6 +1942,9 @@
       <c r="D33" t="s">
         <v>11</v>
       </c>
+      <c r="F33" t="s">
+        <v>276</v>
+      </c>
       <c r="L33" t="s">
         <v>14</v>
       </c>
@@ -1860,6 +1962,9 @@
       <c r="D34" t="s">
         <v>10</v>
       </c>
+      <c r="F34" t="s">
+        <v>276</v>
+      </c>
       <c r="L34" t="s">
         <v>14</v>
       </c>
@@ -1877,6 +1982,9 @@
       <c r="D35" t="s">
         <v>10</v>
       </c>
+      <c r="F35" t="s">
+        <v>276</v>
+      </c>
       <c r="L35" t="s">
         <v>14</v>
       </c>
@@ -1894,6 +2002,9 @@
       <c r="D36" t="s">
         <v>10</v>
       </c>
+      <c r="F36" t="s">
+        <v>276</v>
+      </c>
       <c r="L36" t="s">
         <v>14</v>
       </c>
@@ -1911,6 +2022,9 @@
       <c r="D37" t="s">
         <v>10</v>
       </c>
+      <c r="F37" t="s">
+        <v>276</v>
+      </c>
       <c r="L37" t="s">
         <v>14</v>
       </c>
@@ -1928,6 +2042,9 @@
       <c r="D38" t="s">
         <v>10</v>
       </c>
+      <c r="F38" t="s">
+        <v>276</v>
+      </c>
       <c r="L38" t="s">
         <v>14</v>
       </c>
@@ -1945,6 +2062,9 @@
       <c r="D39" t="s">
         <v>10</v>
       </c>
+      <c r="F39" t="s">
+        <v>276</v>
+      </c>
       <c r="L39" t="s">
         <v>14</v>
       </c>
@@ -1962,6 +2082,9 @@
       <c r="D40" t="s">
         <v>10</v>
       </c>
+      <c r="F40" t="s">
+        <v>276</v>
+      </c>
       <c r="L40" t="s">
         <v>14</v>
       </c>
@@ -1979,6 +2102,9 @@
       <c r="D41" t="s">
         <v>10</v>
       </c>
+      <c r="F41" t="s">
+        <v>276</v>
+      </c>
       <c r="L41" t="s">
         <v>14</v>
       </c>
@@ -1996,6 +2122,9 @@
       <c r="D42" t="s">
         <v>10</v>
       </c>
+      <c r="F42" t="s">
+        <v>276</v>
+      </c>
       <c r="L42" t="s">
         <v>14</v>
       </c>
@@ -2013,6 +2142,9 @@
       <c r="D43" t="s">
         <v>10</v>
       </c>
+      <c r="F43" t="s">
+        <v>276</v>
+      </c>
       <c r="L43" t="s">
         <v>14</v>
       </c>
@@ -2030,6 +2162,9 @@
       <c r="D44" t="s">
         <v>10</v>
       </c>
+      <c r="F44" t="s">
+        <v>276</v>
+      </c>
       <c r="L44" t="s">
         <v>14</v>
       </c>
@@ -2047,6 +2182,9 @@
       <c r="D45" t="s">
         <v>10</v>
       </c>
+      <c r="F45" t="s">
+        <v>276</v>
+      </c>
       <c r="L45" t="s">
         <v>14</v>
       </c>
@@ -2064,6 +2202,9 @@
       <c r="D46" t="s">
         <v>11</v>
       </c>
+      <c r="F46" t="s">
+        <v>276</v>
+      </c>
       <c r="L46" t="s">
         <v>14</v>
       </c>
@@ -2081,6 +2222,9 @@
       <c r="D47" t="s">
         <v>11</v>
       </c>
+      <c r="F47" t="s">
+        <v>276</v>
+      </c>
       <c r="L47" t="s">
         <v>14</v>
       </c>
@@ -2098,6 +2242,9 @@
       <c r="D48" t="s">
         <v>11</v>
       </c>
+      <c r="F48" t="s">
+        <v>276</v>
+      </c>
       <c r="L48" t="s">
         <v>14</v>
       </c>
@@ -2115,6 +2262,9 @@
       <c r="D49" t="s">
         <v>11</v>
       </c>
+      <c r="F49" t="s">
+        <v>276</v>
+      </c>
       <c r="L49" t="s">
         <v>14</v>
       </c>
@@ -2132,6 +2282,9 @@
       <c r="D50" t="s">
         <v>11</v>
       </c>
+      <c r="F50" t="s">
+        <v>276</v>
+      </c>
       <c r="L50" t="s">
         <v>14</v>
       </c>
@@ -2149,6 +2302,9 @@
       <c r="D51" t="s">
         <v>11</v>
       </c>
+      <c r="F51" t="s">
+        <v>276</v>
+      </c>
       <c r="L51" t="s">
         <v>14</v>
       </c>
@@ -2166,6 +2322,9 @@
       <c r="D52" t="s">
         <v>11</v>
       </c>
+      <c r="F52" t="s">
+        <v>276</v>
+      </c>
       <c r="L52" t="s">
         <v>14</v>
       </c>
@@ -2183,6 +2342,9 @@
       <c r="D53" t="s">
         <v>11</v>
       </c>
+      <c r="F53" t="s">
+        <v>276</v>
+      </c>
       <c r="L53" t="s">
         <v>14</v>
       </c>
@@ -2200,6 +2362,9 @@
       <c r="D54" t="s">
         <v>11</v>
       </c>
+      <c r="F54" t="s">
+        <v>276</v>
+      </c>
       <c r="L54" t="s">
         <v>14</v>
       </c>
@@ -2217,6 +2382,9 @@
       <c r="D55" t="s">
         <v>11</v>
       </c>
+      <c r="F55" t="s">
+        <v>276</v>
+      </c>
       <c r="L55" t="s">
         <v>14</v>
       </c>
@@ -2234,6 +2402,9 @@
       <c r="D56" t="s">
         <v>11</v>
       </c>
+      <c r="F56" t="s">
+        <v>276</v>
+      </c>
       <c r="L56" t="s">
         <v>14</v>
       </c>
@@ -2251,6 +2422,9 @@
       <c r="D57" t="s">
         <v>11</v>
       </c>
+      <c r="F57" t="s">
+        <v>276</v>
+      </c>
       <c r="L57" t="s">
         <v>14</v>
       </c>
@@ -2268,6 +2442,9 @@
       <c r="D58" t="s">
         <v>11</v>
       </c>
+      <c r="F58" t="s">
+        <v>276</v>
+      </c>
       <c r="L58" t="s">
         <v>14</v>
       </c>
@@ -2285,6 +2462,9 @@
       <c r="D59" t="s">
         <v>11</v>
       </c>
+      <c r="F59" t="s">
+        <v>276</v>
+      </c>
       <c r="L59" t="s">
         <v>14</v>
       </c>
@@ -2302,6 +2482,9 @@
       <c r="D60" t="s">
         <v>11</v>
       </c>
+      <c r="F60" t="s">
+        <v>276</v>
+      </c>
       <c r="L60" t="s">
         <v>14</v>
       </c>
@@ -2319,6 +2502,9 @@
       <c r="D61" t="s">
         <v>11</v>
       </c>
+      <c r="F61" t="s">
+        <v>276</v>
+      </c>
       <c r="L61" t="s">
         <v>14</v>
       </c>
@@ -2336,6 +2522,9 @@
       <c r="D62" t="s">
         <v>11</v>
       </c>
+      <c r="F62" t="s">
+        <v>276</v>
+      </c>
       <c r="L62" t="s">
         <v>14</v>
       </c>
@@ -2353,6 +2542,9 @@
       <c r="D63" t="s">
         <v>11</v>
       </c>
+      <c r="F63" t="s">
+        <v>276</v>
+      </c>
       <c r="L63" t="s">
         <v>14</v>
       </c>
@@ -2370,6 +2562,9 @@
       <c r="D64" t="s">
         <v>11</v>
       </c>
+      <c r="F64" t="s">
+        <v>276</v>
+      </c>
       <c r="L64" t="s">
         <v>14</v>
       </c>
@@ -2387,6 +2582,9 @@
       <c r="D65" t="s">
         <v>11</v>
       </c>
+      <c r="F65" t="s">
+        <v>276</v>
+      </c>
       <c r="L65" t="s">
         <v>14</v>
       </c>
@@ -2404,6 +2602,9 @@
       <c r="D66" t="s">
         <v>10</v>
       </c>
+      <c r="F66" t="s">
+        <v>276</v>
+      </c>
       <c r="L66" t="s">
         <v>14</v>
       </c>
@@ -2421,6 +2622,9 @@
       <c r="D67" t="s">
         <v>10</v>
       </c>
+      <c r="F67" t="s">
+        <v>276</v>
+      </c>
       <c r="L67" t="s">
         <v>14</v>
       </c>
@@ -2438,6 +2642,9 @@
       <c r="D68" t="s">
         <v>10</v>
       </c>
+      <c r="F68" t="s">
+        <v>276</v>
+      </c>
       <c r="L68" t="s">
         <v>14</v>
       </c>
@@ -2455,6 +2662,9 @@
       <c r="D69" t="s">
         <v>10</v>
       </c>
+      <c r="F69" t="s">
+        <v>276</v>
+      </c>
       <c r="L69" t="s">
         <v>14</v>
       </c>
@@ -2472,6 +2682,9 @@
       <c r="D70" t="s">
         <v>10</v>
       </c>
+      <c r="F70" t="s">
+        <v>276</v>
+      </c>
       <c r="L70" t="s">
         <v>14</v>
       </c>
@@ -2489,6 +2702,9 @@
       <c r="D71" t="s">
         <v>10</v>
       </c>
+      <c r="F71" t="s">
+        <v>276</v>
+      </c>
       <c r="L71" t="s">
         <v>14</v>
       </c>
@@ -2506,6 +2722,9 @@
       <c r="D72" t="s">
         <v>10</v>
       </c>
+      <c r="F72" t="s">
+        <v>276</v>
+      </c>
       <c r="L72" t="s">
         <v>14</v>
       </c>
@@ -2523,6 +2742,9 @@
       <c r="D73" t="s">
         <v>10</v>
       </c>
+      <c r="F73" t="s">
+        <v>276</v>
+      </c>
       <c r="L73" t="s">
         <v>14</v>
       </c>
@@ -2540,6 +2762,9 @@
       <c r="D74" t="s">
         <v>10</v>
       </c>
+      <c r="F74" t="s">
+        <v>276</v>
+      </c>
       <c r="L74" t="s">
         <v>14</v>
       </c>
@@ -2557,6 +2782,9 @@
       <c r="D75" t="s">
         <v>10</v>
       </c>
+      <c r="F75" t="s">
+        <v>276</v>
+      </c>
       <c r="L75" t="s">
         <v>14</v>
       </c>
@@ -2574,6 +2802,9 @@
       <c r="D76" t="s">
         <v>10</v>
       </c>
+      <c r="F76" t="s">
+        <v>276</v>
+      </c>
       <c r="L76" t="s">
         <v>14</v>
       </c>
@@ -2591,6 +2822,9 @@
       <c r="D77" t="s">
         <v>10</v>
       </c>
+      <c r="F77" t="s">
+        <v>276</v>
+      </c>
       <c r="L77" t="s">
         <v>14</v>
       </c>
@@ -2608,6 +2842,9 @@
       <c r="D78" t="s">
         <v>11</v>
       </c>
+      <c r="F78" t="s">
+        <v>276</v>
+      </c>
       <c r="L78" t="s">
         <v>14</v>
       </c>
@@ -2625,6 +2862,9 @@
       <c r="D79" t="s">
         <v>11</v>
       </c>
+      <c r="F79" t="s">
+        <v>276</v>
+      </c>
       <c r="L79" t="s">
         <v>14</v>
       </c>
@@ -2642,6 +2882,9 @@
       <c r="D80" t="s">
         <v>11</v>
       </c>
+      <c r="F80" t="s">
+        <v>276</v>
+      </c>
       <c r="L80" t="s">
         <v>14</v>
       </c>
@@ -2659,6 +2902,9 @@
       <c r="D81" t="s">
         <v>11</v>
       </c>
+      <c r="F81" t="s">
+        <v>276</v>
+      </c>
       <c r="L81" t="s">
         <v>14</v>
       </c>
@@ -2676,6 +2922,9 @@
       <c r="D82" t="s">
         <v>11</v>
       </c>
+      <c r="F82" t="s">
+        <v>276</v>
+      </c>
       <c r="L82" t="s">
         <v>14</v>
       </c>
@@ -2693,6 +2942,9 @@
       <c r="D83" t="s">
         <v>11</v>
       </c>
+      <c r="F83" t="s">
+        <v>276</v>
+      </c>
       <c r="L83" t="s">
         <v>14</v>
       </c>
@@ -2710,6 +2962,9 @@
       <c r="D84" t="s">
         <v>11</v>
       </c>
+      <c r="F84" t="s">
+        <v>276</v>
+      </c>
       <c r="L84" t="s">
         <v>14</v>
       </c>
@@ -2727,6 +2982,9 @@
       <c r="D85" t="s">
         <v>11</v>
       </c>
+      <c r="F85" t="s">
+        <v>276</v>
+      </c>
       <c r="L85" t="s">
         <v>14</v>
       </c>
@@ -2744,6 +3002,9 @@
       <c r="D86" t="s">
         <v>11</v>
       </c>
+      <c r="F86" t="s">
+        <v>276</v>
+      </c>
       <c r="L86" t="s">
         <v>14</v>
       </c>
@@ -2761,6 +3022,9 @@
       <c r="D87" t="s">
         <v>11</v>
       </c>
+      <c r="F87" t="s">
+        <v>276</v>
+      </c>
       <c r="L87" t="s">
         <v>14</v>
       </c>
@@ -2778,6 +3042,9 @@
       <c r="D88" t="s">
         <v>11</v>
       </c>
+      <c r="F88" t="s">
+        <v>276</v>
+      </c>
       <c r="L88" t="s">
         <v>14</v>
       </c>
@@ -2795,6 +3062,9 @@
       <c r="D89" t="s">
         <v>11</v>
       </c>
+      <c r="F89" t="s">
+        <v>276</v>
+      </c>
       <c r="L89" t="s">
         <v>14</v>
       </c>
@@ -2812,6 +3082,9 @@
       <c r="D90" t="s">
         <v>11</v>
       </c>
+      <c r="F90" t="s">
+        <v>276</v>
+      </c>
       <c r="L90" t="s">
         <v>14</v>
       </c>
@@ -2829,6 +3102,9 @@
       <c r="D91" t="s">
         <v>11</v>
       </c>
+      <c r="F91" t="s">
+        <v>276</v>
+      </c>
       <c r="L91" t="s">
         <v>14</v>
       </c>
@@ -2846,6 +3122,9 @@
       <c r="D92" t="s">
         <v>11</v>
       </c>
+      <c r="F92" t="s">
+        <v>276</v>
+      </c>
       <c r="L92" t="s">
         <v>14</v>
       </c>
@@ -2863,6 +3142,9 @@
       <c r="D93" t="s">
         <v>11</v>
       </c>
+      <c r="F93" t="s">
+        <v>276</v>
+      </c>
       <c r="L93" t="s">
         <v>14</v>
       </c>
@@ -2880,6 +3162,9 @@
       <c r="D94" t="s">
         <v>11</v>
       </c>
+      <c r="F94" t="s">
+        <v>276</v>
+      </c>
       <c r="L94" t="s">
         <v>273</v>
       </c>
@@ -2897,6 +3182,9 @@
       <c r="D95" t="s">
         <v>11</v>
       </c>
+      <c r="F95" t="s">
+        <v>276</v>
+      </c>
       <c r="L95" t="s">
         <v>14</v>
       </c>
@@ -2914,6 +3202,9 @@
       <c r="D96" t="s">
         <v>11</v>
       </c>
+      <c r="F96" t="s">
+        <v>276</v>
+      </c>
       <c r="L96" t="s">
         <v>14</v>
       </c>
@@ -2931,6 +3222,9 @@
       <c r="D97" t="s">
         <v>11</v>
       </c>
+      <c r="F97" t="s">
+        <v>276</v>
+      </c>
       <c r="L97" t="s">
         <v>14</v>
       </c>
@@ -4526,8 +4820,17 @@
       <c r="E143">
         <v>2031111</v>
       </c>
+      <c r="F143" t="s">
+        <v>277</v>
+      </c>
       <c r="H143" t="s">
         <v>274</v>
+      </c>
+      <c r="I143" t="s">
+        <v>22</v>
+      </c>
+      <c r="K143" t="s">
+        <v>23</v>
       </c>
       <c r="L143" t="s">
         <v>272</v>
@@ -4549,8 +4852,17 @@
       <c r="E144">
         <v>2031111</v>
       </c>
+      <c r="F144" t="s">
+        <v>277</v>
+      </c>
       <c r="H144" t="s">
         <v>274</v>
+      </c>
+      <c r="I144" t="s">
+        <v>22</v>
+      </c>
+      <c r="K144" t="s">
+        <v>23</v>
       </c>
       <c r="L144" t="s">
         <v>272</v>
@@ -4572,8 +4884,17 @@
       <c r="E145">
         <v>2031111</v>
       </c>
+      <c r="F145" t="s">
+        <v>277</v>
+      </c>
       <c r="H145" t="s">
         <v>274</v>
+      </c>
+      <c r="I145" t="s">
+        <v>22</v>
+      </c>
+      <c r="K145" t="s">
+        <v>23</v>
       </c>
       <c r="L145" t="s">
         <v>272</v>
@@ -4595,8 +4916,17 @@
       <c r="E146">
         <v>2031111</v>
       </c>
+      <c r="F146" t="s">
+        <v>277</v>
+      </c>
       <c r="H146" t="s">
         <v>274</v>
+      </c>
+      <c r="I146" t="s">
+        <v>22</v>
+      </c>
+      <c r="K146" t="s">
+        <v>23</v>
       </c>
       <c r="L146" t="s">
         <v>272</v>
@@ -4618,8 +4948,17 @@
       <c r="E147">
         <v>2031111</v>
       </c>
+      <c r="F147" t="s">
+        <v>277</v>
+      </c>
       <c r="H147" t="s">
         <v>274</v>
+      </c>
+      <c r="I147" t="s">
+        <v>22</v>
+      </c>
+      <c r="K147" t="s">
+        <v>23</v>
       </c>
       <c r="L147" t="s">
         <v>272</v>
@@ -4641,8 +4980,17 @@
       <c r="E148">
         <v>2031111</v>
       </c>
+      <c r="F148" t="s">
+        <v>277</v>
+      </c>
       <c r="H148" t="s">
         <v>274</v>
+      </c>
+      <c r="I148" t="s">
+        <v>22</v>
+      </c>
+      <c r="K148" t="s">
+        <v>23</v>
       </c>
       <c r="L148" t="s">
         <v>272</v>
@@ -4664,8 +5012,17 @@
       <c r="E149">
         <v>2031111</v>
       </c>
+      <c r="F149" t="s">
+        <v>277</v>
+      </c>
       <c r="H149" t="s">
         <v>275</v>
+      </c>
+      <c r="I149" t="s">
+        <v>22</v>
+      </c>
+      <c r="K149" t="s">
+        <v>23</v>
       </c>
       <c r="L149" t="s">
         <v>272</v>
@@ -4687,8 +5044,17 @@
       <c r="E150">
         <v>2031111</v>
       </c>
+      <c r="F150" t="s">
+        <v>277</v>
+      </c>
       <c r="H150" t="s">
         <v>274</v>
+      </c>
+      <c r="I150" t="s">
+        <v>22</v>
+      </c>
+      <c r="K150" t="s">
+        <v>23</v>
       </c>
       <c r="L150" t="s">
         <v>272</v>
@@ -4710,8 +5076,17 @@
       <c r="E151">
         <v>2031111</v>
       </c>
+      <c r="F151" t="s">
+        <v>277</v>
+      </c>
       <c r="H151" t="s">
         <v>275</v>
+      </c>
+      <c r="I151" t="s">
+        <v>22</v>
+      </c>
+      <c r="K151" t="s">
+        <v>23</v>
       </c>
       <c r="L151" t="s">
         <v>272</v>
@@ -4733,8 +5108,17 @@
       <c r="E152">
         <v>2031111</v>
       </c>
+      <c r="F152" t="s">
+        <v>277</v>
+      </c>
       <c r="H152" t="s">
         <v>274</v>
+      </c>
+      <c r="I152" t="s">
+        <v>22</v>
+      </c>
+      <c r="K152" t="s">
+        <v>23</v>
       </c>
       <c r="L152" t="s">
         <v>272</v>
@@ -4756,8 +5140,17 @@
       <c r="E153">
         <v>2031111</v>
       </c>
+      <c r="F153" t="s">
+        <v>277</v>
+      </c>
       <c r="H153" t="s">
         <v>274</v>
+      </c>
+      <c r="I153" t="s">
+        <v>22</v>
+      </c>
+      <c r="K153" t="s">
+        <v>23</v>
       </c>
       <c r="L153" t="s">
         <v>272</v>
@@ -4779,8 +5172,17 @@
       <c r="E154">
         <v>2031111</v>
       </c>
+      <c r="F154" t="s">
+        <v>277</v>
+      </c>
       <c r="H154" t="s">
         <v>274</v>
+      </c>
+      <c r="I154" t="s">
+        <v>22</v>
+      </c>
+      <c r="K154" t="s">
+        <v>23</v>
       </c>
       <c r="L154" t="s">
         <v>272</v>
@@ -4802,8 +5204,17 @@
       <c r="E155">
         <v>2031111</v>
       </c>
+      <c r="F155" t="s">
+        <v>277</v>
+      </c>
       <c r="H155" t="s">
         <v>274</v>
+      </c>
+      <c r="I155" t="s">
+        <v>22</v>
+      </c>
+      <c r="K155" t="s">
+        <v>23</v>
       </c>
       <c r="L155" t="s">
         <v>272</v>
@@ -4825,8 +5236,17 @@
       <c r="E156">
         <v>2031111</v>
       </c>
+      <c r="F156" t="s">
+        <v>277</v>
+      </c>
       <c r="H156" t="s">
         <v>274</v>
+      </c>
+      <c r="I156" t="s">
+        <v>22</v>
+      </c>
+      <c r="K156" t="s">
+        <v>23</v>
       </c>
       <c r="L156" t="s">
         <v>272</v>
@@ -4848,8 +5268,17 @@
       <c r="E157">
         <v>2031111</v>
       </c>
+      <c r="F157" t="s">
+        <v>277</v>
+      </c>
       <c r="H157" t="s">
         <v>274</v>
+      </c>
+      <c r="I157" t="s">
+        <v>22</v>
+      </c>
+      <c r="K157" t="s">
+        <v>23</v>
       </c>
       <c r="L157" t="s">
         <v>272</v>
@@ -4871,8 +5300,17 @@
       <c r="E158">
         <v>2031111</v>
       </c>
+      <c r="F158" t="s">
+        <v>277</v>
+      </c>
       <c r="H158" t="s">
         <v>274</v>
+      </c>
+      <c r="I158" t="s">
+        <v>22</v>
+      </c>
+      <c r="K158" t="s">
+        <v>23</v>
       </c>
       <c r="L158" t="s">
         <v>272</v>
@@ -4894,8 +5332,17 @@
       <c r="E159">
         <v>2031111</v>
       </c>
+      <c r="F159" t="s">
+        <v>277</v>
+      </c>
       <c r="H159" t="s">
         <v>274</v>
+      </c>
+      <c r="I159" t="s">
+        <v>22</v>
+      </c>
+      <c r="K159" t="s">
+        <v>23</v>
       </c>
       <c r="L159" t="s">
         <v>272</v>
@@ -4917,8 +5364,17 @@
       <c r="E160">
         <v>2031111</v>
       </c>
+      <c r="F160" t="s">
+        <v>277</v>
+      </c>
       <c r="H160" t="s">
         <v>274</v>
+      </c>
+      <c r="I160" t="s">
+        <v>22</v>
+      </c>
+      <c r="K160" t="s">
+        <v>23</v>
       </c>
       <c r="L160" t="s">
         <v>272</v>
@@ -4940,8 +5396,17 @@
       <c r="E161">
         <v>2031111</v>
       </c>
+      <c r="F161" t="s">
+        <v>277</v>
+      </c>
       <c r="H161" t="s">
         <v>274</v>
+      </c>
+      <c r="I161" t="s">
+        <v>22</v>
+      </c>
+      <c r="K161" t="s">
+        <v>23</v>
       </c>
       <c r="L161" t="s">
         <v>272</v>
@@ -4963,8 +5428,17 @@
       <c r="E162">
         <v>2031111</v>
       </c>
+      <c r="F162" t="s">
+        <v>277</v>
+      </c>
       <c r="H162" t="s">
         <v>274</v>
+      </c>
+      <c r="I162" t="s">
+        <v>22</v>
+      </c>
+      <c r="K162" t="s">
+        <v>23</v>
       </c>
       <c r="L162" t="s">
         <v>272</v>
@@ -4986,8 +5460,17 @@
       <c r="E163">
         <v>2031111</v>
       </c>
+      <c r="F163" t="s">
+        <v>277</v>
+      </c>
       <c r="H163" t="s">
         <v>274</v>
+      </c>
+      <c r="I163" t="s">
+        <v>22</v>
+      </c>
+      <c r="K163" t="s">
+        <v>23</v>
       </c>
       <c r="L163" t="s">
         <v>272</v>
@@ -5009,8 +5492,17 @@
       <c r="E164">
         <v>2031111</v>
       </c>
+      <c r="F164" t="s">
+        <v>277</v>
+      </c>
       <c r="H164" t="s">
         <v>274</v>
+      </c>
+      <c r="I164" t="s">
+        <v>22</v>
+      </c>
+      <c r="K164" t="s">
+        <v>23</v>
       </c>
       <c r="L164" t="s">
         <v>272</v>
@@ -5032,8 +5524,17 @@
       <c r="E165">
         <v>2031111</v>
       </c>
+      <c r="F165" t="s">
+        <v>277</v>
+      </c>
       <c r="H165" t="s">
         <v>274</v>
+      </c>
+      <c r="I165" t="s">
+        <v>22</v>
+      </c>
+      <c r="K165" t="s">
+        <v>23</v>
       </c>
       <c r="L165" t="s">
         <v>272</v>
@@ -5055,8 +5556,17 @@
       <c r="E166">
         <v>2031111</v>
       </c>
+      <c r="F166" t="s">
+        <v>277</v>
+      </c>
       <c r="H166" t="s">
         <v>275</v>
+      </c>
+      <c r="I166" t="s">
+        <v>22</v>
+      </c>
+      <c r="K166" t="s">
+        <v>23</v>
       </c>
       <c r="L166" t="s">
         <v>272</v>
@@ -5078,8 +5588,17 @@
       <c r="E167">
         <v>2031111</v>
       </c>
+      <c r="F167" t="s">
+        <v>277</v>
+      </c>
       <c r="H167" t="s">
         <v>274</v>
+      </c>
+      <c r="I167" t="s">
+        <v>22</v>
+      </c>
+      <c r="K167" t="s">
+        <v>23</v>
       </c>
       <c r="L167" t="s">
         <v>272</v>
@@ -5101,8 +5620,17 @@
       <c r="E168">
         <v>2031111</v>
       </c>
+      <c r="F168" t="s">
+        <v>277</v>
+      </c>
       <c r="H168" t="s">
         <v>275</v>
+      </c>
+      <c r="I168" t="s">
+        <v>22</v>
+      </c>
+      <c r="K168" t="s">
+        <v>23</v>
       </c>
       <c r="L168" t="s">
         <v>272</v>
@@ -5124,8 +5652,17 @@
       <c r="E169">
         <v>2031111</v>
       </c>
+      <c r="F169" t="s">
+        <v>277</v>
+      </c>
       <c r="H169" t="s">
         <v>274</v>
+      </c>
+      <c r="I169" t="s">
+        <v>22</v>
+      </c>
+      <c r="K169" t="s">
+        <v>23</v>
       </c>
       <c r="L169" t="s">
         <v>272</v>
@@ -5147,8 +5684,17 @@
       <c r="E170">
         <v>2031111</v>
       </c>
+      <c r="F170" t="s">
+        <v>277</v>
+      </c>
       <c r="H170" t="s">
         <v>275</v>
+      </c>
+      <c r="I170" t="s">
+        <v>22</v>
+      </c>
+      <c r="K170" t="s">
+        <v>23</v>
       </c>
       <c r="L170" t="s">
         <v>272</v>
@@ -5170,8 +5716,17 @@
       <c r="E171">
         <v>2031111</v>
       </c>
+      <c r="F171" t="s">
+        <v>277</v>
+      </c>
       <c r="H171" t="s">
         <v>275</v>
+      </c>
+      <c r="I171" t="s">
+        <v>22</v>
+      </c>
+      <c r="K171" t="s">
+        <v>23</v>
       </c>
       <c r="L171" t="s">
         <v>272</v>
@@ -5193,8 +5748,17 @@
       <c r="E172">
         <v>2031111</v>
       </c>
+      <c r="F172" t="s">
+        <v>277</v>
+      </c>
       <c r="H172" t="s">
         <v>275</v>
+      </c>
+      <c r="I172" t="s">
+        <v>22</v>
+      </c>
+      <c r="K172" t="s">
+        <v>23</v>
       </c>
       <c r="L172" t="s">
         <v>272</v>
@@ -5216,8 +5780,17 @@
       <c r="E173">
         <v>2031111</v>
       </c>
+      <c r="F173" t="s">
+        <v>277</v>
+      </c>
       <c r="H173" t="s">
         <v>274</v>
+      </c>
+      <c r="I173" t="s">
+        <v>22</v>
+      </c>
+      <c r="K173" t="s">
+        <v>23</v>
       </c>
       <c r="L173" t="s">
         <v>272</v>
@@ -5239,8 +5812,17 @@
       <c r="E174">
         <v>2031111</v>
       </c>
+      <c r="F174" t="s">
+        <v>277</v>
+      </c>
       <c r="H174" t="s">
         <v>275</v>
+      </c>
+      <c r="I174" t="s">
+        <v>22</v>
+      </c>
+      <c r="K174" t="s">
+        <v>23</v>
       </c>
       <c r="L174" t="s">
         <v>272</v>
@@ -5262,8 +5844,17 @@
       <c r="E175">
         <v>2031111</v>
       </c>
+      <c r="F175" t="s">
+        <v>277</v>
+      </c>
       <c r="H175" t="s">
         <v>275</v>
+      </c>
+      <c r="I175" t="s">
+        <v>22</v>
+      </c>
+      <c r="K175" t="s">
+        <v>23</v>
       </c>
       <c r="L175" t="s">
         <v>272</v>
@@ -5285,8 +5876,17 @@
       <c r="E176">
         <v>2031111</v>
       </c>
+      <c r="F176" t="s">
+        <v>277</v>
+      </c>
       <c r="H176" t="s">
         <v>274</v>
+      </c>
+      <c r="I176" t="s">
+        <v>22</v>
+      </c>
+      <c r="K176" t="s">
+        <v>23</v>
       </c>
       <c r="L176" t="s">
         <v>272</v>
@@ -5308,8 +5908,17 @@
       <c r="E177">
         <v>2031111</v>
       </c>
+      <c r="F177" t="s">
+        <v>277</v>
+      </c>
       <c r="H177" t="s">
         <v>275</v>
+      </c>
+      <c r="I177" t="s">
+        <v>22</v>
+      </c>
+      <c r="K177" t="s">
+        <v>23</v>
       </c>
       <c r="L177" t="s">
         <v>272</v>
@@ -5331,8 +5940,17 @@
       <c r="E178">
         <v>2031111</v>
       </c>
+      <c r="F178" t="s">
+        <v>277</v>
+      </c>
       <c r="H178" t="s">
         <v>274</v>
+      </c>
+      <c r="I178" t="s">
+        <v>22</v>
+      </c>
+      <c r="K178" t="s">
+        <v>23</v>
       </c>
       <c r="L178" t="s">
         <v>272</v>
@@ -5354,8 +5972,17 @@
       <c r="E179">
         <v>2031111</v>
       </c>
+      <c r="F179" t="s">
+        <v>277</v>
+      </c>
       <c r="H179" t="s">
         <v>274</v>
+      </c>
+      <c r="I179" t="s">
+        <v>22</v>
+      </c>
+      <c r="K179" t="s">
+        <v>23</v>
       </c>
       <c r="L179" t="s">
         <v>272</v>
@@ -5377,8 +6004,17 @@
       <c r="E180">
         <v>2031111</v>
       </c>
+      <c r="F180" t="s">
+        <v>277</v>
+      </c>
       <c r="H180" t="s">
         <v>274</v>
+      </c>
+      <c r="I180" t="s">
+        <v>22</v>
+      </c>
+      <c r="K180" t="s">
+        <v>23</v>
       </c>
       <c r="L180" t="s">
         <v>272</v>
@@ -5400,8 +6036,17 @@
       <c r="E181">
         <v>2031111</v>
       </c>
+      <c r="F181" t="s">
+        <v>277</v>
+      </c>
       <c r="H181" t="s">
         <v>274</v>
+      </c>
+      <c r="I181" t="s">
+        <v>22</v>
+      </c>
+      <c r="K181" t="s">
+        <v>23</v>
       </c>
       <c r="L181" t="s">
         <v>272</v>
@@ -5423,8 +6068,17 @@
       <c r="E182">
         <v>2031111</v>
       </c>
+      <c r="F182" t="s">
+        <v>277</v>
+      </c>
       <c r="H182" t="s">
         <v>274</v>
+      </c>
+      <c r="I182" t="s">
+        <v>22</v>
+      </c>
+      <c r="K182" t="s">
+        <v>23</v>
       </c>
       <c r="L182" t="s">
         <v>272</v>
@@ -5446,8 +6100,17 @@
       <c r="E183">
         <v>2031111</v>
       </c>
+      <c r="F183" t="s">
+        <v>277</v>
+      </c>
       <c r="H183" t="s">
         <v>274</v>
+      </c>
+      <c r="I183" t="s">
+        <v>22</v>
+      </c>
+      <c r="K183" t="s">
+        <v>23</v>
       </c>
       <c r="L183" t="s">
         <v>272</v>
@@ -5469,8 +6132,17 @@
       <c r="E184">
         <v>2031111</v>
       </c>
+      <c r="F184" t="s">
+        <v>277</v>
+      </c>
       <c r="H184" t="s">
         <v>274</v>
+      </c>
+      <c r="I184" t="s">
+        <v>22</v>
+      </c>
+      <c r="K184" t="s">
+        <v>23</v>
       </c>
       <c r="L184" t="s">
         <v>272</v>
@@ -5492,8 +6164,17 @@
       <c r="E185">
         <v>2031111</v>
       </c>
+      <c r="F185" t="s">
+        <v>277</v>
+      </c>
       <c r="H185" t="s">
         <v>274</v>
+      </c>
+      <c r="I185" t="s">
+        <v>22</v>
+      </c>
+      <c r="K185" t="s">
+        <v>23</v>
       </c>
       <c r="L185" t="s">
         <v>272</v>
@@ -5515,8 +6196,17 @@
       <c r="E186">
         <v>2031111</v>
       </c>
+      <c r="F186" t="s">
+        <v>277</v>
+      </c>
       <c r="H186" t="s">
         <v>274</v>
+      </c>
+      <c r="I186" t="s">
+        <v>22</v>
+      </c>
+      <c r="K186" t="s">
+        <v>23</v>
       </c>
       <c r="L186" t="s">
         <v>272</v>
@@ -5538,8 +6228,17 @@
       <c r="E187">
         <v>2031111</v>
       </c>
+      <c r="F187" t="s">
+        <v>277</v>
+      </c>
       <c r="H187" t="s">
         <v>274</v>
+      </c>
+      <c r="I187" t="s">
+        <v>22</v>
+      </c>
+      <c r="K187" t="s">
+        <v>23</v>
       </c>
       <c r="L187" t="s">
         <v>272</v>
@@ -5561,8 +6260,17 @@
       <c r="E188">
         <v>2031111</v>
       </c>
+      <c r="F188" t="s">
+        <v>277</v>
+      </c>
       <c r="H188" t="s">
         <v>274</v>
+      </c>
+      <c r="I188" t="s">
+        <v>22</v>
+      </c>
+      <c r="K188" t="s">
+        <v>23</v>
       </c>
       <c r="L188" t="s">
         <v>272</v>
@@ -5584,8 +6292,17 @@
       <c r="E189">
         <v>2031111</v>
       </c>
+      <c r="F189" t="s">
+        <v>277</v>
+      </c>
       <c r="H189" t="s">
         <v>274</v>
+      </c>
+      <c r="I189" t="s">
+        <v>22</v>
+      </c>
+      <c r="K189" t="s">
+        <v>23</v>
       </c>
       <c r="L189" t="s">
         <v>272</v>
@@ -5607,8 +6324,17 @@
       <c r="E190">
         <v>2031111</v>
       </c>
+      <c r="F190" t="s">
+        <v>277</v>
+      </c>
       <c r="H190" t="s">
         <v>274</v>
+      </c>
+      <c r="I190" t="s">
+        <v>22</v>
+      </c>
+      <c r="K190" t="s">
+        <v>23</v>
       </c>
       <c r="L190" t="s">
         <v>272</v>
@@ -5630,8 +6356,17 @@
       <c r="E191">
         <v>2031111</v>
       </c>
+      <c r="F191" t="s">
+        <v>277</v>
+      </c>
       <c r="H191" t="s">
         <v>274</v>
+      </c>
+      <c r="I191" t="s">
+        <v>22</v>
+      </c>
+      <c r="K191" t="s">
+        <v>23</v>
       </c>
       <c r="L191" t="s">
         <v>272</v>
@@ -5653,8 +6388,17 @@
       <c r="E192">
         <v>2031111</v>
       </c>
+      <c r="F192" t="s">
+        <v>277</v>
+      </c>
       <c r="H192" t="s">
         <v>274</v>
+      </c>
+      <c r="I192" t="s">
+        <v>22</v>
+      </c>
+      <c r="K192" t="s">
+        <v>23</v>
       </c>
       <c r="L192" t="s">
         <v>272</v>
@@ -5676,8 +6420,17 @@
       <c r="E193">
         <v>2031111</v>
       </c>
+      <c r="F193" t="s">
+        <v>277</v>
+      </c>
       <c r="H193" t="s">
         <v>274</v>
+      </c>
+      <c r="I193" t="s">
+        <v>22</v>
+      </c>
+      <c r="K193" t="s">
+        <v>23</v>
       </c>
       <c r="L193" t="s">
         <v>272</v>
@@ -5699,8 +6452,17 @@
       <c r="E194">
         <v>2031111</v>
       </c>
+      <c r="F194" t="s">
+        <v>277</v>
+      </c>
       <c r="H194" t="s">
         <v>274</v>
+      </c>
+      <c r="I194" t="s">
+        <v>22</v>
+      </c>
+      <c r="K194" t="s">
+        <v>23</v>
       </c>
       <c r="L194" t="s">
         <v>272</v>
@@ -5722,8 +6484,17 @@
       <c r="E195">
         <v>2031111</v>
       </c>
+      <c r="F195" t="s">
+        <v>277</v>
+      </c>
       <c r="H195" t="s">
         <v>274</v>
+      </c>
+      <c r="I195" t="s">
+        <v>22</v>
+      </c>
+      <c r="K195" t="s">
+        <v>23</v>
       </c>
       <c r="L195" t="s">
         <v>272</v>
@@ -5745,8 +6516,17 @@
       <c r="E196">
         <v>2031111</v>
       </c>
+      <c r="F196" t="s">
+        <v>277</v>
+      </c>
       <c r="H196" t="s">
         <v>274</v>
+      </c>
+      <c r="I196" t="s">
+        <v>22</v>
+      </c>
+      <c r="K196" t="s">
+        <v>23</v>
       </c>
       <c r="L196" t="s">
         <v>272</v>
@@ -5768,8 +6548,17 @@
       <c r="E197">
         <v>2031111</v>
       </c>
+      <c r="F197" t="s">
+        <v>277</v>
+      </c>
       <c r="H197" t="s">
         <v>274</v>
+      </c>
+      <c r="I197" t="s">
+        <v>22</v>
+      </c>
+      <c r="K197" t="s">
+        <v>23</v>
       </c>
       <c r="L197" t="s">
         <v>272</v>
@@ -5791,8 +6580,17 @@
       <c r="E198">
         <v>2031111</v>
       </c>
+      <c r="F198" t="s">
+        <v>277</v>
+      </c>
       <c r="H198" t="s">
         <v>274</v>
+      </c>
+      <c r="I198" t="s">
+        <v>22</v>
+      </c>
+      <c r="K198" t="s">
+        <v>23</v>
       </c>
       <c r="L198" t="s">
         <v>272</v>
@@ -5814,8 +6612,17 @@
       <c r="E199">
         <v>2023111</v>
       </c>
+      <c r="F199" t="s">
+        <v>277</v>
+      </c>
       <c r="H199" t="s">
         <v>274</v>
+      </c>
+      <c r="I199" t="s">
+        <v>22</v>
+      </c>
+      <c r="K199" t="s">
+        <v>23</v>
       </c>
       <c r="L199" t="s">
         <v>272</v>
@@ -5837,8 +6644,17 @@
       <c r="E200">
         <v>2023111</v>
       </c>
+      <c r="F200" t="s">
+        <v>277</v>
+      </c>
       <c r="H200" t="s">
         <v>274</v>
+      </c>
+      <c r="I200" t="s">
+        <v>22</v>
+      </c>
+      <c r="K200" t="s">
+        <v>23</v>
       </c>
       <c r="L200" t="s">
         <v>272</v>
@@ -5860,8 +6676,17 @@
       <c r="E201">
         <v>2031111</v>
       </c>
+      <c r="F201" t="s">
+        <v>277</v>
+      </c>
       <c r="H201" t="s">
         <v>274</v>
+      </c>
+      <c r="I201" t="s">
+        <v>22</v>
+      </c>
+      <c r="K201" t="s">
+        <v>23</v>
       </c>
       <c r="L201" t="s">
         <v>272</v>
@@ -5883,8 +6708,17 @@
       <c r="E202">
         <v>2031111</v>
       </c>
+      <c r="F202" t="s">
+        <v>277</v>
+      </c>
       <c r="H202" t="s">
         <v>274</v>
+      </c>
+      <c r="I202" t="s">
+        <v>22</v>
+      </c>
+      <c r="K202" t="s">
+        <v>23</v>
       </c>
       <c r="L202" t="s">
         <v>272</v>
@@ -5906,8 +6740,17 @@
       <c r="E203">
         <v>2031111</v>
       </c>
+      <c r="F203" t="s">
+        <v>277</v>
+      </c>
       <c r="H203" t="s">
         <v>274</v>
+      </c>
+      <c r="I203" t="s">
+        <v>22</v>
+      </c>
+      <c r="K203" t="s">
+        <v>23</v>
       </c>
       <c r="L203" t="s">
         <v>272</v>
@@ -5929,8 +6772,17 @@
       <c r="E204">
         <v>2031111</v>
       </c>
+      <c r="F204" t="s">
+        <v>277</v>
+      </c>
       <c r="H204" t="s">
         <v>274</v>
+      </c>
+      <c r="I204" t="s">
+        <v>22</v>
+      </c>
+      <c r="K204" t="s">
+        <v>23</v>
       </c>
       <c r="L204" t="s">
         <v>272</v>
@@ -5952,8 +6804,17 @@
       <c r="E205">
         <v>2031111</v>
       </c>
+      <c r="F205" t="s">
+        <v>277</v>
+      </c>
       <c r="H205" t="s">
         <v>274</v>
+      </c>
+      <c r="I205" t="s">
+        <v>22</v>
+      </c>
+      <c r="K205" t="s">
+        <v>23</v>
       </c>
       <c r="L205" t="s">
         <v>272</v>
@@ -5975,8 +6836,17 @@
       <c r="E206">
         <v>2031111</v>
       </c>
+      <c r="F206" t="s">
+        <v>277</v>
+      </c>
       <c r="H206" t="s">
         <v>274</v>
+      </c>
+      <c r="I206" t="s">
+        <v>22</v>
+      </c>
+      <c r="K206" t="s">
+        <v>23</v>
       </c>
       <c r="L206" t="s">
         <v>272</v>
@@ -5998,8 +6868,17 @@
       <c r="E207">
         <v>2031111</v>
       </c>
+      <c r="F207" t="s">
+        <v>277</v>
+      </c>
       <c r="H207" t="s">
         <v>274</v>
+      </c>
+      <c r="I207" t="s">
+        <v>22</v>
+      </c>
+      <c r="K207" t="s">
+        <v>23</v>
       </c>
       <c r="L207" t="s">
         <v>272</v>
@@ -6021,8 +6900,17 @@
       <c r="E208">
         <v>2031111</v>
       </c>
+      <c r="F208" t="s">
+        <v>277</v>
+      </c>
       <c r="H208" t="s">
         <v>274</v>
+      </c>
+      <c r="I208" t="s">
+        <v>22</v>
+      </c>
+      <c r="K208" t="s">
+        <v>23</v>
       </c>
       <c r="L208" t="s">
         <v>272</v>
@@ -6044,8 +6932,17 @@
       <c r="E209">
         <v>2031111</v>
       </c>
+      <c r="F209" t="s">
+        <v>277</v>
+      </c>
       <c r="H209" t="s">
         <v>274</v>
+      </c>
+      <c r="I209" t="s">
+        <v>22</v>
+      </c>
+      <c r="K209" t="s">
+        <v>23</v>
       </c>
       <c r="L209" t="s">
         <v>272</v>
@@ -6067,8 +6964,17 @@
       <c r="E210">
         <v>2031111</v>
       </c>
+      <c r="F210" t="s">
+        <v>277</v>
+      </c>
       <c r="H210" t="s">
         <v>274</v>
+      </c>
+      <c r="I210" t="s">
+        <v>22</v>
+      </c>
+      <c r="K210" t="s">
+        <v>23</v>
       </c>
       <c r="L210" t="s">
         <v>272</v>
@@ -6090,8 +6996,17 @@
       <c r="E211">
         <v>2031111</v>
       </c>
+      <c r="F211" t="s">
+        <v>277</v>
+      </c>
       <c r="H211" t="s">
         <v>274</v>
+      </c>
+      <c r="I211" t="s">
+        <v>22</v>
+      </c>
+      <c r="K211" t="s">
+        <v>23</v>
       </c>
       <c r="L211" t="s">
         <v>272</v>
@@ -6113,8 +7028,17 @@
       <c r="E212">
         <v>2031111</v>
       </c>
+      <c r="F212" t="s">
+        <v>277</v>
+      </c>
       <c r="H212" t="s">
         <v>274</v>
+      </c>
+      <c r="I212" t="s">
+        <v>22</v>
+      </c>
+      <c r="K212" t="s">
+        <v>23</v>
       </c>
       <c r="L212" t="s">
         <v>272</v>
@@ -6136,8 +7060,17 @@
       <c r="E213">
         <v>2031111</v>
       </c>
+      <c r="F213" t="s">
+        <v>277</v>
+      </c>
       <c r="H213" t="s">
         <v>274</v>
+      </c>
+      <c r="I213" t="s">
+        <v>22</v>
+      </c>
+      <c r="K213" t="s">
+        <v>23</v>
       </c>
       <c r="L213" t="s">
         <v>272</v>
@@ -6159,8 +7092,17 @@
       <c r="E214">
         <v>2031111</v>
       </c>
+      <c r="F214" t="s">
+        <v>277</v>
+      </c>
       <c r="H214" t="s">
         <v>274</v>
+      </c>
+      <c r="I214" t="s">
+        <v>22</v>
+      </c>
+      <c r="K214" t="s">
+        <v>23</v>
       </c>
       <c r="L214" t="s">
         <v>272</v>
@@ -6182,8 +7124,17 @@
       <c r="E215">
         <v>2031111</v>
       </c>
+      <c r="F215" t="s">
+        <v>277</v>
+      </c>
       <c r="H215" t="s">
         <v>275</v>
+      </c>
+      <c r="I215" t="s">
+        <v>22</v>
+      </c>
+      <c r="K215" t="s">
+        <v>23</v>
       </c>
       <c r="L215" t="s">
         <v>272</v>
@@ -6205,8 +7156,17 @@
       <c r="E216">
         <v>2031111</v>
       </c>
+      <c r="F216" t="s">
+        <v>277</v>
+      </c>
       <c r="H216" t="s">
         <v>274</v>
+      </c>
+      <c r="I216" t="s">
+        <v>22</v>
+      </c>
+      <c r="K216" t="s">
+        <v>23</v>
       </c>
       <c r="L216" t="s">
         <v>272</v>
@@ -6228,8 +7188,17 @@
       <c r="E217">
         <v>2031111</v>
       </c>
+      <c r="F217" t="s">
+        <v>277</v>
+      </c>
       <c r="H217" t="s">
         <v>275</v>
+      </c>
+      <c r="I217" t="s">
+        <v>22</v>
+      </c>
+      <c r="K217" t="s">
+        <v>23</v>
       </c>
       <c r="L217" t="s">
         <v>272</v>
@@ -6251,8 +7220,17 @@
       <c r="E218">
         <v>2031111</v>
       </c>
+      <c r="F218" t="s">
+        <v>277</v>
+      </c>
       <c r="H218" t="s">
         <v>275</v>
+      </c>
+      <c r="I218" t="s">
+        <v>22</v>
+      </c>
+      <c r="K218" t="s">
+        <v>23</v>
       </c>
       <c r="L218" t="s">
         <v>272</v>
@@ -6274,8 +7252,17 @@
       <c r="E219">
         <v>2031111</v>
       </c>
+      <c r="F219" t="s">
+        <v>277</v>
+      </c>
       <c r="H219" t="s">
         <v>274</v>
+      </c>
+      <c r="I219" t="s">
+        <v>22</v>
+      </c>
+      <c r="K219" t="s">
+        <v>23</v>
       </c>
       <c r="L219" t="s">
         <v>272</v>
@@ -6297,8 +7284,17 @@
       <c r="E220">
         <v>2031111</v>
       </c>
+      <c r="F220" t="s">
+        <v>277</v>
+      </c>
       <c r="H220" t="s">
         <v>275</v>
+      </c>
+      <c r="I220" t="s">
+        <v>22</v>
+      </c>
+      <c r="K220" t="s">
+        <v>23</v>
       </c>
       <c r="L220" t="s">
         <v>272</v>
@@ -6317,6 +7313,15 @@
       <c r="D221" t="s">
         <v>10</v>
       </c>
+      <c r="F221" t="s">
+        <v>277</v>
+      </c>
+      <c r="I221" t="s">
+        <v>22</v>
+      </c>
+      <c r="K221" t="s">
+        <v>23</v>
+      </c>
       <c r="L221" t="s">
         <v>272</v>
       </c>
@@ -6334,6 +7339,15 @@
       <c r="D222" t="s">
         <v>10</v>
       </c>
+      <c r="F222" t="s">
+        <v>277</v>
+      </c>
+      <c r="I222" t="s">
+        <v>22</v>
+      </c>
+      <c r="K222" t="s">
+        <v>23</v>
+      </c>
       <c r="L222" t="s">
         <v>272</v>
       </c>
@@ -6351,6 +7365,15 @@
       <c r="D223" t="s">
         <v>10</v>
       </c>
+      <c r="F223" t="s">
+        <v>277</v>
+      </c>
+      <c r="I223" t="s">
+        <v>22</v>
+      </c>
+      <c r="K223" t="s">
+        <v>23</v>
+      </c>
       <c r="L223" t="s">
         <v>272</v>
       </c>
@@ -6368,6 +7391,15 @@
       <c r="D224" t="s">
         <v>10</v>
       </c>
+      <c r="F224" t="s">
+        <v>277</v>
+      </c>
+      <c r="I224" t="s">
+        <v>22</v>
+      </c>
+      <c r="K224" t="s">
+        <v>23</v>
+      </c>
       <c r="L224" t="s">
         <v>272</v>
       </c>
@@ -6385,6 +7417,15 @@
       <c r="D225" t="s">
         <v>10</v>
       </c>
+      <c r="F225" t="s">
+        <v>277</v>
+      </c>
+      <c r="I225" t="s">
+        <v>22</v>
+      </c>
+      <c r="K225" t="s">
+        <v>23</v>
+      </c>
       <c r="L225" t="s">
         <v>272</v>
       </c>
@@ -6402,6 +7443,15 @@
       <c r="D226" t="s">
         <v>10</v>
       </c>
+      <c r="F226" t="s">
+        <v>277</v>
+      </c>
+      <c r="I226" t="s">
+        <v>22</v>
+      </c>
+      <c r="K226" t="s">
+        <v>23</v>
+      </c>
       <c r="L226" t="s">
         <v>272</v>
       </c>
@@ -6422,8 +7472,17 @@
       <c r="E227">
         <v>2031111</v>
       </c>
+      <c r="F227" t="s">
+        <v>277</v>
+      </c>
       <c r="H227" t="s">
         <v>274</v>
+      </c>
+      <c r="I227" t="s">
+        <v>22</v>
+      </c>
+      <c r="K227" t="s">
+        <v>23</v>
       </c>
       <c r="L227" t="s">
         <v>272</v>
@@ -6445,8 +7504,17 @@
       <c r="E228">
         <v>2031111</v>
       </c>
+      <c r="F228" t="s">
+        <v>277</v>
+      </c>
       <c r="H228" t="s">
         <v>275</v>
+      </c>
+      <c r="I228" t="s">
+        <v>22</v>
+      </c>
+      <c r="K228" t="s">
+        <v>23</v>
       </c>
       <c r="L228" t="s">
         <v>272</v>
@@ -6468,8 +7536,17 @@
       <c r="E229">
         <v>2031111</v>
       </c>
+      <c r="F229" t="s">
+        <v>277</v>
+      </c>
       <c r="H229" t="s">
         <v>274</v>
+      </c>
+      <c r="I229" t="s">
+        <v>22</v>
+      </c>
+      <c r="K229" t="s">
+        <v>23</v>
       </c>
       <c r="L229" t="s">
         <v>272</v>
@@ -6491,8 +7568,17 @@
       <c r="E230">
         <v>2031111</v>
       </c>
+      <c r="F230" t="s">
+        <v>277</v>
+      </c>
       <c r="H230" t="s">
         <v>274</v>
+      </c>
+      <c r="I230" t="s">
+        <v>22</v>
+      </c>
+      <c r="K230" t="s">
+        <v>23</v>
       </c>
       <c r="L230" t="s">
         <v>272</v>
@@ -6514,8 +7600,17 @@
       <c r="E231">
         <v>2031111</v>
       </c>
+      <c r="F231" t="s">
+        <v>277</v>
+      </c>
       <c r="H231" t="s">
         <v>274</v>
+      </c>
+      <c r="I231" t="s">
+        <v>22</v>
+      </c>
+      <c r="K231" t="s">
+        <v>23</v>
       </c>
       <c r="L231" t="s">
         <v>272</v>
@@ -6537,8 +7632,17 @@
       <c r="E232">
         <v>2031111</v>
       </c>
+      <c r="F232" t="s">
+        <v>277</v>
+      </c>
       <c r="H232" t="s">
         <v>274</v>
+      </c>
+      <c r="I232" t="s">
+        <v>22</v>
+      </c>
+      <c r="K232" t="s">
+        <v>23</v>
       </c>
       <c r="L232" t="s">
         <v>272</v>
@@ -6560,8 +7664,17 @@
       <c r="E233">
         <v>2031111</v>
       </c>
+      <c r="F233" t="s">
+        <v>277</v>
+      </c>
       <c r="H233" t="s">
         <v>274</v>
+      </c>
+      <c r="I233" t="s">
+        <v>22</v>
+      </c>
+      <c r="K233" t="s">
+        <v>23</v>
       </c>
       <c r="L233" t="s">
         <v>272</v>
@@ -6583,8 +7696,17 @@
       <c r="E234">
         <v>2031111</v>
       </c>
+      <c r="F234" t="s">
+        <v>277</v>
+      </c>
       <c r="H234" t="s">
         <v>274</v>
+      </c>
+      <c r="I234" t="s">
+        <v>22</v>
+      </c>
+      <c r="K234" t="s">
+        <v>23</v>
       </c>
       <c r="L234" t="s">
         <v>272</v>
@@ -6606,8 +7728,17 @@
       <c r="E235">
         <v>2031111</v>
       </c>
+      <c r="F235" t="s">
+        <v>277</v>
+      </c>
       <c r="H235" t="s">
         <v>274</v>
+      </c>
+      <c r="I235" t="s">
+        <v>22</v>
+      </c>
+      <c r="K235" t="s">
+        <v>23</v>
       </c>
       <c r="L235" t="s">
         <v>272</v>
@@ -6629,8 +7760,17 @@
       <c r="E236">
         <v>2031111</v>
       </c>
+      <c r="F236" t="s">
+        <v>277</v>
+      </c>
       <c r="H236" t="s">
         <v>275</v>
+      </c>
+      <c r="I236" t="s">
+        <v>22</v>
+      </c>
+      <c r="K236" t="s">
+        <v>23</v>
       </c>
       <c r="L236" t="s">
         <v>272</v>
@@ -6652,8 +7792,17 @@
       <c r="E237">
         <v>2031111</v>
       </c>
+      <c r="F237" t="s">
+        <v>277</v>
+      </c>
       <c r="H237" t="s">
         <v>274</v>
+      </c>
+      <c r="I237" t="s">
+        <v>22</v>
+      </c>
+      <c r="K237" t="s">
+        <v>23</v>
       </c>
       <c r="L237" t="s">
         <v>272</v>
@@ -6675,8 +7824,17 @@
       <c r="E238">
         <v>2031111</v>
       </c>
+      <c r="F238" t="s">
+        <v>277</v>
+      </c>
       <c r="H238" t="s">
         <v>274</v>
+      </c>
+      <c r="I238" t="s">
+        <v>22</v>
+      </c>
+      <c r="K238" t="s">
+        <v>23</v>
       </c>
       <c r="L238" t="s">
         <v>272</v>
@@ -6698,8 +7856,17 @@
       <c r="E239">
         <v>2031111</v>
       </c>
+      <c r="F239" t="s">
+        <v>277</v>
+      </c>
       <c r="H239" t="s">
         <v>274</v>
+      </c>
+      <c r="I239" t="s">
+        <v>22</v>
+      </c>
+      <c r="K239" t="s">
+        <v>23</v>
       </c>
       <c r="L239" t="s">
         <v>272</v>
@@ -6721,8 +7888,17 @@
       <c r="E240">
         <v>2031111</v>
       </c>
+      <c r="F240" t="s">
+        <v>277</v>
+      </c>
       <c r="H240" t="s">
         <v>275</v>
+      </c>
+      <c r="I240" t="s">
+        <v>22</v>
+      </c>
+      <c r="K240" t="s">
+        <v>23</v>
       </c>
       <c r="L240" t="s">
         <v>272</v>
@@ -6744,8 +7920,17 @@
       <c r="E241">
         <v>2031111</v>
       </c>
+      <c r="F241" t="s">
+        <v>277</v>
+      </c>
       <c r="H241" t="s">
         <v>274</v>
+      </c>
+      <c r="I241" t="s">
+        <v>22</v>
+      </c>
+      <c r="K241" t="s">
+        <v>23</v>
       </c>
       <c r="L241" t="s">
         <v>272</v>
@@ -6767,8 +7952,17 @@
       <c r="E242">
         <v>2031111</v>
       </c>
+      <c r="F242" t="s">
+        <v>277</v>
+      </c>
       <c r="H242" t="s">
         <v>274</v>
+      </c>
+      <c r="I242" t="s">
+        <v>22</v>
+      </c>
+      <c r="K242" t="s">
+        <v>23</v>
       </c>
       <c r="L242" t="s">
         <v>272</v>
@@ -6787,6 +7981,15 @@
       <c r="D243" t="s">
         <v>11</v>
       </c>
+      <c r="F243" t="s">
+        <v>277</v>
+      </c>
+      <c r="I243" t="s">
+        <v>22</v>
+      </c>
+      <c r="K243" t="s">
+        <v>23</v>
+      </c>
       <c r="L243" t="s">
         <v>272</v>
       </c>
@@ -6804,6 +8007,15 @@
       <c r="D244" t="s">
         <v>11</v>
       </c>
+      <c r="F244" t="s">
+        <v>277</v>
+      </c>
+      <c r="I244" t="s">
+        <v>22</v>
+      </c>
+      <c r="K244" t="s">
+        <v>23</v>
+      </c>
       <c r="L244" t="s">
         <v>272</v>
       </c>
@@ -6821,6 +8033,15 @@
       <c r="D245" t="s">
         <v>11</v>
       </c>
+      <c r="F245" t="s">
+        <v>277</v>
+      </c>
+      <c r="I245" t="s">
+        <v>22</v>
+      </c>
+      <c r="K245" t="s">
+        <v>23</v>
+      </c>
       <c r="L245" t="s">
         <v>272</v>
       </c>
@@ -6838,6 +8059,15 @@
       <c r="D246" t="s">
         <v>11</v>
       </c>
+      <c r="F246" t="s">
+        <v>277</v>
+      </c>
+      <c r="I246" t="s">
+        <v>22</v>
+      </c>
+      <c r="K246" t="s">
+        <v>23</v>
+      </c>
       <c r="L246" t="s">
         <v>272</v>
       </c>
@@ -6858,8 +8088,17 @@
       <c r="E247">
         <v>2031111</v>
       </c>
+      <c r="F247" t="s">
+        <v>277</v>
+      </c>
       <c r="H247" t="s">
         <v>274</v>
+      </c>
+      <c r="I247" t="s">
+        <v>22</v>
+      </c>
+      <c r="K247" t="s">
+        <v>23</v>
       </c>
       <c r="L247" t="s">
         <v>272</v>
@@ -6881,8 +8120,17 @@
       <c r="E248">
         <v>2031111</v>
       </c>
+      <c r="F248" t="s">
+        <v>277</v>
+      </c>
       <c r="H248" t="s">
         <v>274</v>
+      </c>
+      <c r="I248" t="s">
+        <v>22</v>
+      </c>
+      <c r="K248" t="s">
+        <v>23</v>
       </c>
       <c r="L248" t="s">
         <v>272</v>
@@ -6904,8 +8152,17 @@
       <c r="E249">
         <v>2031111</v>
       </c>
+      <c r="F249" t="s">
+        <v>277</v>
+      </c>
       <c r="H249" t="s">
         <v>274</v>
+      </c>
+      <c r="I249" t="s">
+        <v>22</v>
+      </c>
+      <c r="K249" t="s">
+        <v>23</v>
       </c>
       <c r="L249" t="s">
         <v>272</v>
@@ -6927,8 +8184,17 @@
       <c r="E250">
         <v>2031111</v>
       </c>
+      <c r="F250" t="s">
+        <v>277</v>
+      </c>
       <c r="H250" t="s">
         <v>274</v>
+      </c>
+      <c r="I250" t="s">
+        <v>22</v>
+      </c>
+      <c r="K250" t="s">
+        <v>23</v>
       </c>
       <c r="L250" t="s">
         <v>272</v>

</xml_diff>

<commit_message>
fixed daily measurement file format issue
</commit_message>
<xml_diff>
--- a/data/dna/dna_metadata.xlsx
+++ b/data/dna/dna_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/moorea_symbiotic_exchange_2023/data/dna/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7724F164-D563-D84F-AFE5-7CB279B88C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4286425C-0778-FA4D-8F29-CD0916EC7727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3540" yWindow="820" windowWidth="24220" windowHeight="17560" xr2:uid="{6B87E6CE-126B-8B47-B516-351EEAF1A0B4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1751" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1761" uniqueCount="279">
   <si>
     <t>sample_id</t>
   </si>
@@ -870,6 +870,9 @@
   </si>
   <si>
     <t>Isotopes</t>
+  </si>
+  <si>
+    <t>Box 3</t>
   </si>
 </sst>
 </file>
@@ -1255,8 +1258,8 @@
   <dimension ref="A1:L250"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A211" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F242" sqref="F242"/>
+      <pane ySplit="1" topLeftCell="A216" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D233" sqref="D233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4818,7 +4821,7 @@
         <v>10</v>
       </c>
       <c r="E143">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F143" t="s">
         <v>277</v>
@@ -4850,7 +4853,7 @@
         <v>10</v>
       </c>
       <c r="E144">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F144" t="s">
         <v>277</v>
@@ -4882,7 +4885,7 @@
         <v>10</v>
       </c>
       <c r="E145">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F145" t="s">
         <v>277</v>
@@ -4914,7 +4917,7 @@
         <v>10</v>
       </c>
       <c r="E146">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F146" t="s">
         <v>277</v>
@@ -4946,7 +4949,7 @@
         <v>10</v>
       </c>
       <c r="E147">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F147" t="s">
         <v>277</v>
@@ -4978,7 +4981,7 @@
         <v>10</v>
       </c>
       <c r="E148">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F148" t="s">
         <v>277</v>
@@ -5010,7 +5013,7 @@
         <v>10</v>
       </c>
       <c r="E149">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F149" t="s">
         <v>277</v>
@@ -5042,7 +5045,7 @@
         <v>10</v>
       </c>
       <c r="E150">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F150" t="s">
         <v>277</v>
@@ -5074,7 +5077,7 @@
         <v>10</v>
       </c>
       <c r="E151">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F151" t="s">
         <v>277</v>
@@ -5106,7 +5109,7 @@
         <v>10</v>
       </c>
       <c r="E152">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F152" t="s">
         <v>277</v>
@@ -5138,7 +5141,7 @@
         <v>10</v>
       </c>
       <c r="E153">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F153" t="s">
         <v>277</v>
@@ -5170,7 +5173,7 @@
         <v>10</v>
       </c>
       <c r="E154">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F154" t="s">
         <v>277</v>
@@ -5202,7 +5205,7 @@
         <v>10</v>
       </c>
       <c r="E155">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F155" t="s">
         <v>277</v>
@@ -5234,7 +5237,7 @@
         <v>10</v>
       </c>
       <c r="E156">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F156" t="s">
         <v>277</v>
@@ -5266,7 +5269,7 @@
         <v>10</v>
       </c>
       <c r="E157">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F157" t="s">
         <v>277</v>
@@ -5298,7 +5301,7 @@
         <v>11</v>
       </c>
       <c r="E158">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F158" t="s">
         <v>277</v>
@@ -5330,7 +5333,7 @@
         <v>11</v>
       </c>
       <c r="E159">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F159" t="s">
         <v>277</v>
@@ -5362,7 +5365,7 @@
         <v>11</v>
       </c>
       <c r="E160">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F160" t="s">
         <v>277</v>
@@ -5394,7 +5397,7 @@
         <v>11</v>
       </c>
       <c r="E161">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F161" t="s">
         <v>277</v>
@@ -5426,7 +5429,7 @@
         <v>11</v>
       </c>
       <c r="E162">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F162" t="s">
         <v>277</v>
@@ -5458,7 +5461,7 @@
         <v>11</v>
       </c>
       <c r="E163">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F163" t="s">
         <v>277</v>
@@ -5490,7 +5493,7 @@
         <v>11</v>
       </c>
       <c r="E164">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F164" t="s">
         <v>277</v>
@@ -5522,7 +5525,7 @@
         <v>11</v>
       </c>
       <c r="E165">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F165" t="s">
         <v>277</v>
@@ -5554,7 +5557,7 @@
         <v>11</v>
       </c>
       <c r="E166">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F166" t="s">
         <v>277</v>
@@ -5586,7 +5589,7 @@
         <v>11</v>
       </c>
       <c r="E167">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F167" t="s">
         <v>277</v>
@@ -5618,7 +5621,7 @@
         <v>11</v>
       </c>
       <c r="E168">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F168" t="s">
         <v>277</v>
@@ -5650,7 +5653,7 @@
         <v>11</v>
       </c>
       <c r="E169">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F169" t="s">
         <v>277</v>
@@ -5682,7 +5685,7 @@
         <v>11</v>
       </c>
       <c r="E170">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F170" t="s">
         <v>277</v>
@@ -5714,7 +5717,7 @@
         <v>11</v>
       </c>
       <c r="E171">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F171" t="s">
         <v>277</v>
@@ -5746,7 +5749,7 @@
         <v>11</v>
       </c>
       <c r="E172">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F172" t="s">
         <v>277</v>
@@ -5778,7 +5781,7 @@
         <v>11</v>
       </c>
       <c r="E173">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F173" t="s">
         <v>277</v>
@@ -5810,7 +5813,7 @@
         <v>11</v>
       </c>
       <c r="E174">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F174" t="s">
         <v>277</v>
@@ -5842,7 +5845,7 @@
         <v>11</v>
       </c>
       <c r="E175">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F175" t="s">
         <v>277</v>
@@ -5874,7 +5877,7 @@
         <v>11</v>
       </c>
       <c r="E176">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F176" t="s">
         <v>277</v>
@@ -5906,7 +5909,7 @@
         <v>11</v>
       </c>
       <c r="E177">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F177" t="s">
         <v>277</v>
@@ -5938,7 +5941,7 @@
         <v>11</v>
       </c>
       <c r="E178">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F178" t="s">
         <v>277</v>
@@ -5970,7 +5973,7 @@
         <v>10</v>
       </c>
       <c r="E179">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F179" t="s">
         <v>277</v>
@@ -6002,7 +6005,7 @@
         <v>10</v>
       </c>
       <c r="E180">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F180" t="s">
         <v>277</v>
@@ -6034,7 +6037,7 @@
         <v>10</v>
       </c>
       <c r="E181">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F181" t="s">
         <v>277</v>
@@ -6066,7 +6069,7 @@
         <v>10</v>
       </c>
       <c r="E182">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F182" t="s">
         <v>277</v>
@@ -6098,7 +6101,7 @@
         <v>10</v>
       </c>
       <c r="E183">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F183" t="s">
         <v>277</v>
@@ -6130,7 +6133,7 @@
         <v>10</v>
       </c>
       <c r="E184">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F184" t="s">
         <v>277</v>
@@ -6162,7 +6165,7 @@
         <v>10</v>
       </c>
       <c r="E185">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F185" t="s">
         <v>277</v>
@@ -6194,7 +6197,7 @@
         <v>10</v>
       </c>
       <c r="E186">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F186" t="s">
         <v>277</v>
@@ -6226,7 +6229,7 @@
         <v>10</v>
       </c>
       <c r="E187">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F187" t="s">
         <v>277</v>
@@ -6258,7 +6261,7 @@
         <v>10</v>
       </c>
       <c r="E188">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F188" t="s">
         <v>277</v>
@@ -6290,7 +6293,7 @@
         <v>10</v>
       </c>
       <c r="E189">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F189" t="s">
         <v>277</v>
@@ -6322,7 +6325,7 @@
         <v>10</v>
       </c>
       <c r="E190">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F190" t="s">
         <v>277</v>
@@ -6354,7 +6357,7 @@
         <v>10</v>
       </c>
       <c r="E191">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F191" t="s">
         <v>277</v>
@@ -6386,7 +6389,7 @@
         <v>10</v>
       </c>
       <c r="E192">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F192" t="s">
         <v>277</v>
@@ -6418,7 +6421,7 @@
         <v>10</v>
       </c>
       <c r="E193">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F193" t="s">
         <v>277</v>
@@ -6450,7 +6453,7 @@
         <v>11</v>
       </c>
       <c r="E194">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F194" t="s">
         <v>277</v>
@@ -6482,7 +6485,7 @@
         <v>11</v>
       </c>
       <c r="E195">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F195" t="s">
         <v>277</v>
@@ -6514,7 +6517,7 @@
         <v>11</v>
       </c>
       <c r="E196">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F196" t="s">
         <v>277</v>
@@ -6546,7 +6549,7 @@
         <v>11</v>
       </c>
       <c r="E197">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F197" t="s">
         <v>277</v>
@@ -6578,7 +6581,7 @@
         <v>11</v>
       </c>
       <c r="E198">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F198" t="s">
         <v>277</v>
@@ -6610,7 +6613,7 @@
         <v>11</v>
       </c>
       <c r="E199">
-        <v>2023111</v>
+        <v>20231111</v>
       </c>
       <c r="F199" t="s">
         <v>277</v>
@@ -6642,7 +6645,7 @@
         <v>11</v>
       </c>
       <c r="E200">
-        <v>2023111</v>
+        <v>20231111</v>
       </c>
       <c r="F200" t="s">
         <v>277</v>
@@ -6674,7 +6677,7 @@
         <v>11</v>
       </c>
       <c r="E201">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F201" t="s">
         <v>277</v>
@@ -6706,7 +6709,7 @@
         <v>11</v>
       </c>
       <c r="E202">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F202" t="s">
         <v>277</v>
@@ -6738,7 +6741,7 @@
         <v>11</v>
       </c>
       <c r="E203">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F203" t="s">
         <v>277</v>
@@ -6770,7 +6773,7 @@
         <v>11</v>
       </c>
       <c r="E204">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F204" t="s">
         <v>277</v>
@@ -6802,7 +6805,7 @@
         <v>11</v>
       </c>
       <c r="E205">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F205" t="s">
         <v>277</v>
@@ -6834,7 +6837,7 @@
         <v>11</v>
       </c>
       <c r="E206">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F206" t="s">
         <v>277</v>
@@ -6866,7 +6869,7 @@
         <v>11</v>
       </c>
       <c r="E207">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F207" t="s">
         <v>277</v>
@@ -6898,7 +6901,7 @@
         <v>11</v>
       </c>
       <c r="E208">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F208" t="s">
         <v>277</v>
@@ -6930,7 +6933,7 @@
         <v>11</v>
       </c>
       <c r="E209">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F209" t="s">
         <v>277</v>
@@ -6962,7 +6965,7 @@
         <v>11</v>
       </c>
       <c r="E210">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F210" t="s">
         <v>277</v>
@@ -6994,7 +6997,7 @@
         <v>11</v>
       </c>
       <c r="E211">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F211" t="s">
         <v>277</v>
@@ -7026,7 +7029,7 @@
         <v>11</v>
       </c>
       <c r="E212">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F212" t="s">
         <v>277</v>
@@ -7058,7 +7061,7 @@
         <v>11</v>
       </c>
       <c r="E213">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F213" t="s">
         <v>277</v>
@@ -7090,7 +7093,7 @@
         <v>11</v>
       </c>
       <c r="E214">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F214" t="s">
         <v>277</v>
@@ -7122,7 +7125,7 @@
         <v>10</v>
       </c>
       <c r="E215">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F215" t="s">
         <v>277</v>
@@ -7154,7 +7157,7 @@
         <v>10</v>
       </c>
       <c r="E216">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F216" t="s">
         <v>277</v>
@@ -7186,7 +7189,7 @@
         <v>10</v>
       </c>
       <c r="E217">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F217" t="s">
         <v>277</v>
@@ -7218,7 +7221,7 @@
         <v>10</v>
       </c>
       <c r="E218">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F218" t="s">
         <v>277</v>
@@ -7250,7 +7253,7 @@
         <v>10</v>
       </c>
       <c r="E219">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F219" t="s">
         <v>277</v>
@@ -7282,7 +7285,7 @@
         <v>10</v>
       </c>
       <c r="E220">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F220" t="s">
         <v>277</v>
@@ -7313,8 +7316,14 @@
       <c r="D221" t="s">
         <v>10</v>
       </c>
+      <c r="E221">
+        <v>20231112</v>
+      </c>
       <c r="F221" t="s">
         <v>277</v>
+      </c>
+      <c r="H221" t="s">
+        <v>278</v>
       </c>
       <c r="I221" t="s">
         <v>22</v>
@@ -7339,8 +7348,14 @@
       <c r="D222" t="s">
         <v>10</v>
       </c>
+      <c r="E222">
+        <v>20231112</v>
+      </c>
       <c r="F222" t="s">
         <v>277</v>
+      </c>
+      <c r="H222" t="s">
+        <v>278</v>
       </c>
       <c r="I222" t="s">
         <v>22</v>
@@ -7365,8 +7380,14 @@
       <c r="D223" t="s">
         <v>10</v>
       </c>
+      <c r="E223">
+        <v>20231112</v>
+      </c>
       <c r="F223" t="s">
         <v>277</v>
+      </c>
+      <c r="H223" t="s">
+        <v>278</v>
       </c>
       <c r="I223" t="s">
         <v>22</v>
@@ -7391,8 +7412,14 @@
       <c r="D224" t="s">
         <v>10</v>
       </c>
+      <c r="E224">
+        <v>20231112</v>
+      </c>
       <c r="F224" t="s">
         <v>277</v>
+      </c>
+      <c r="H224" t="s">
+        <v>278</v>
       </c>
       <c r="I224" t="s">
         <v>22</v>
@@ -7417,8 +7444,14 @@
       <c r="D225" t="s">
         <v>10</v>
       </c>
+      <c r="E225">
+        <v>20231112</v>
+      </c>
       <c r="F225" t="s">
         <v>277</v>
+      </c>
+      <c r="H225" t="s">
+        <v>278</v>
       </c>
       <c r="I225" t="s">
         <v>22</v>
@@ -7443,8 +7476,14 @@
       <c r="D226" t="s">
         <v>10</v>
       </c>
+      <c r="E226">
+        <v>20231112</v>
+      </c>
       <c r="F226" t="s">
         <v>277</v>
+      </c>
+      <c r="H226" t="s">
+        <v>278</v>
       </c>
       <c r="I226" t="s">
         <v>22</v>
@@ -7470,7 +7509,7 @@
         <v>10</v>
       </c>
       <c r="E227">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F227" t="s">
         <v>277</v>
@@ -7502,7 +7541,7 @@
         <v>10</v>
       </c>
       <c r="E228">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F228" t="s">
         <v>277</v>
@@ -7534,7 +7573,7 @@
         <v>10</v>
       </c>
       <c r="E229">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F229" t="s">
         <v>277</v>
@@ -7566,7 +7605,7 @@
         <v>11</v>
       </c>
       <c r="E230">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F230" t="s">
         <v>277</v>
@@ -7598,7 +7637,7 @@
         <v>11</v>
       </c>
       <c r="E231">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F231" t="s">
         <v>277</v>
@@ -7630,7 +7669,7 @@
         <v>11</v>
       </c>
       <c r="E232">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F232" t="s">
         <v>277</v>
@@ -7662,7 +7701,7 @@
         <v>11</v>
       </c>
       <c r="E233">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F233" t="s">
         <v>277</v>
@@ -7694,7 +7733,7 @@
         <v>11</v>
       </c>
       <c r="E234">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F234" t="s">
         <v>277</v>
@@ -7726,7 +7765,7 @@
         <v>11</v>
       </c>
       <c r="E235">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F235" t="s">
         <v>277</v>
@@ -7758,7 +7797,7 @@
         <v>11</v>
       </c>
       <c r="E236">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F236" t="s">
         <v>277</v>
@@ -7790,7 +7829,7 @@
         <v>11</v>
       </c>
       <c r="E237">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F237" t="s">
         <v>277</v>
@@ -7822,7 +7861,7 @@
         <v>11</v>
       </c>
       <c r="E238">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F238" t="s">
         <v>277</v>
@@ -7854,7 +7893,7 @@
         <v>11</v>
       </c>
       <c r="E239">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F239" t="s">
         <v>277</v>
@@ -7886,7 +7925,7 @@
         <v>11</v>
       </c>
       <c r="E240">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F240" t="s">
         <v>277</v>
@@ -7918,7 +7957,7 @@
         <v>11</v>
       </c>
       <c r="E241">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F241" t="s">
         <v>277</v>
@@ -7950,7 +7989,7 @@
         <v>11</v>
       </c>
       <c r="E242">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F242" t="s">
         <v>277</v>
@@ -7981,8 +8020,14 @@
       <c r="D243" t="s">
         <v>11</v>
       </c>
+      <c r="E243">
+        <v>20231112</v>
+      </c>
       <c r="F243" t="s">
         <v>277</v>
+      </c>
+      <c r="H243" t="s">
+        <v>278</v>
       </c>
       <c r="I243" t="s">
         <v>22</v>
@@ -8007,8 +8052,14 @@
       <c r="D244" t="s">
         <v>11</v>
       </c>
+      <c r="E244">
+        <v>20231112</v>
+      </c>
       <c r="F244" t="s">
         <v>277</v>
+      </c>
+      <c r="H244" t="s">
+        <v>278</v>
       </c>
       <c r="I244" t="s">
         <v>22</v>
@@ -8033,8 +8084,14 @@
       <c r="D245" t="s">
         <v>11</v>
       </c>
+      <c r="E245">
+        <v>20231112</v>
+      </c>
       <c r="F245" t="s">
         <v>277</v>
+      </c>
+      <c r="H245" t="s">
+        <v>278</v>
       </c>
       <c r="I245" t="s">
         <v>22</v>
@@ -8059,8 +8116,14 @@
       <c r="D246" t="s">
         <v>11</v>
       </c>
+      <c r="E246">
+        <v>20231112</v>
+      </c>
       <c r="F246" t="s">
         <v>277</v>
+      </c>
+      <c r="H246" t="s">
+        <v>278</v>
       </c>
       <c r="I246" t="s">
         <v>22</v>
@@ -8086,7 +8149,7 @@
         <v>11</v>
       </c>
       <c r="E247">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F247" t="s">
         <v>277</v>
@@ -8118,7 +8181,7 @@
         <v>11</v>
       </c>
       <c r="E248">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F248" t="s">
         <v>277</v>
@@ -8150,7 +8213,7 @@
         <v>11</v>
       </c>
       <c r="E249">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F249" t="s">
         <v>277</v>
@@ -8182,7 +8245,7 @@
         <v>11</v>
       </c>
       <c r="E250">
-        <v>2031111</v>
+        <v>20231111</v>
       </c>
       <c r="F250" t="s">
         <v>277</v>

</xml_diff>

<commit_message>
updated species ID details
</commit_message>
<xml_diff>
--- a/data/dna/dna_metadata.xlsx
+++ b/data/dna/dna_metadata.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/moorea_symbiotic_exchange_2023/data/dna/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194EA378-2B8C-1B48-8E7D-CA0142B6DF54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1693CF02-ABEE-1A45-A0AE-438E90918C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23500" yWindow="-260" windowWidth="21060" windowHeight="18760" xr2:uid="{6B87E6CE-126B-8B47-B516-351EEAF1A0B4}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{6B87E6CE-126B-8B47-B516-351EEAF1A0B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
+    <sheet name="Totals" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3159" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3181" uniqueCount="418">
   <si>
     <t>sample_id</t>
   </si>
@@ -1251,6 +1252,45 @@
   </si>
   <si>
     <t>27 Dark</t>
+  </si>
+  <si>
+    <t>POCILLOPORA</t>
+  </si>
+  <si>
+    <t>ACROPORA</t>
+  </si>
+  <si>
+    <t>PORITES</t>
+  </si>
+  <si>
+    <t>Adults</t>
+  </si>
+  <si>
+    <t>Recruits</t>
+  </si>
+  <si>
+    <t>evermanni</t>
+  </si>
+  <si>
+    <t>lobata lutea</t>
+  </si>
+  <si>
+    <t>meandrina</t>
+  </si>
+  <si>
+    <t>verrucosa</t>
+  </si>
+  <si>
+    <t>grandis</t>
+  </si>
+  <si>
+    <t>tuahiniensis</t>
+  </si>
+  <si>
+    <t>effusa</t>
+  </si>
+  <si>
+    <t>acuta</t>
   </si>
 </sst>
 </file>
@@ -1378,7 +1418,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1397,6 +1437,8 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1713,11 +1755,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5716CA15-A063-CD4A-965E-FFCB3C4243EA}">
   <dimension ref="A1:X244"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="N41" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="88" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="O191" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R61" sqref="R61"/>
+      <selection pane="bottomRight" activeCell="R93" sqref="R93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15111,4 +15153,224 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED9E7F29-BE4D-B046-8E84-2D8B88558186}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.5" style="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>405</v>
+      </c>
+      <c r="B1" t="s">
+        <v>408</v>
+      </c>
+      <c r="C1" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="19" t="s">
+        <v>412</v>
+      </c>
+      <c r="B2">
+        <f>SUM(Metadata!R141,Metadata!R90)</f>
+        <v>13</v>
+      </c>
+      <c r="C2">
+        <f>SUM(Metadata!R152,Metadata!R101)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="19" t="s">
+        <v>413</v>
+      </c>
+      <c r="B3">
+        <f>SUM(Metadata!R142,Metadata!R91)</f>
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <f>SUM(Metadata!R153,Metadata!R102)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="19" t="s">
+        <v>414</v>
+      </c>
+      <c r="B4">
+        <f>SUM(Metadata!R143,Metadata!R92)</f>
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <f>SUM(Metadata!R154,Metadata!R103)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="19" t="s">
+        <v>415</v>
+      </c>
+      <c r="B5">
+        <f>SUM(Metadata!R144,Metadata!R93)</f>
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <f>SUM(Metadata!R155,Metadata!R104)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="19" t="s">
+        <v>416</v>
+      </c>
+      <c r="B6">
+        <f>SUM(Metadata!R145,Metadata!R94)</f>
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <f>SUM(Metadata!R156,Metadata!R105)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="19" t="s">
+        <v>417</v>
+      </c>
+      <c r="B7">
+        <f>SUM(Metadata!R146,Metadata!R95)</f>
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <f>SUM(Metadata!R157,Metadata!R106)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="19" t="s">
+        <v>406</v>
+      </c>
+      <c r="B9" t="s">
+        <v>408</v>
+      </c>
+      <c r="C9" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="18" t="s">
+        <v>399</v>
+      </c>
+      <c r="B10">
+        <f>SUM(Metadata!S12,Metadata!S61)</f>
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <f>SUM(Metadata!S71,Metadata!S22)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="18" t="s">
+        <v>400</v>
+      </c>
+      <c r="B11">
+        <f>SUM(Metadata!S13,Metadata!S62)</f>
+        <v>13</v>
+      </c>
+      <c r="C11">
+        <f>SUM(Metadata!S72,Metadata!S23)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="18" t="s">
+        <v>401</v>
+      </c>
+      <c r="B12">
+        <f>SUM(Metadata!S14,Metadata!S63)</f>
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <f>SUM(Metadata!S73,Metadata!S24)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="18" t="s">
+        <v>402</v>
+      </c>
+      <c r="B13">
+        <f>SUM(Metadata!S15,Metadata!S64)</f>
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <f>SUM(Metadata!S74,Metadata!S25)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="18" t="s">
+        <v>403</v>
+      </c>
+      <c r="B14">
+        <f>SUM(Metadata!S16,Metadata!S65)</f>
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <f>SUM(Metadata!S75,Metadata!S26)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="19" t="s">
+        <v>407</v>
+      </c>
+      <c r="B16" t="s">
+        <v>408</v>
+      </c>
+      <c r="C16" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="19" t="s">
+        <v>410</v>
+      </c>
+      <c r="B17">
+        <f>SUM(Metadata!R176,Metadata!S224)</f>
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <f>SUM(Metadata!R183,Metadata!S231)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="19" t="s">
+        <v>411</v>
+      </c>
+      <c r="B18">
+        <f>SUM(Metadata!R177,Metadata!S225)</f>
+        <v>25</v>
+      </c>
+      <c r="C18">
+        <f>SUM(Metadata!R184,Metadata!S232)</f>
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>